<commit_message>
Updated explore project & made bug fixes from 04_27 testing
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Packaging_Resources/lib/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Packaging_Resources/lib/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB195E56-540E-4352-9C39-20643A03C131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD3014A-6E6B-4546-9576-1F0D89E3EEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-165" yWindow="90" windowWidth="12030" windowHeight="14940" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="498">
   <si>
     <t>ID</t>
   </si>
@@ -818,15 +818,6 @@
     <t>MainForm</t>
   </si>
   <si>
-    <t>The Importance of Storytelling</t>
-  </si>
-  <si>
-    <t>Storytelling Best Practices</t>
-  </si>
-  <si>
-    <t>Equity and Resilience</t>
-  </si>
-  <si>
     <t>Who are ERB users?</t>
   </si>
   <si>
@@ -848,36 +839,18 @@
     <t>15</t>
   </si>
   <si>
-    <t>Chapter 1 About</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
-    <t>Chapter 2 About</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
-    <t>Chapter 3 About</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
-    <t>Chapter 4 About</t>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
-    <t>Chapter 5 About</t>
-  </si>
-  <si>
-    <t>Team Storytelling</t>
-  </si>
-  <si>
     <t>Goal Setting Scenario</t>
   </si>
   <si>
@@ -896,9 +869,6 @@
     <t>Lay your cards on the table</t>
   </si>
   <si>
-    <t>Sorting indicator cards</t>
-  </si>
-  <si>
     <t>27</t>
   </si>
   <si>
@@ -914,36 +884,12 @@
     <t>29</t>
   </si>
   <si>
-    <t>How have other communities used the ERB tool? Goal setting examples</t>
-  </si>
-  <si>
-    <t>How have other communities used the ERB tool? Activity selection examples</t>
-  </si>
-  <si>
-    <t>Select activities to do in ERB</t>
-  </si>
-  <si>
-    <t>Reflection and next steps (Ch 1)</t>
-  </si>
-  <si>
-    <t>Identify and Diagram Community Connections</t>
-  </si>
-  <si>
     <t>Diagram Community Connections</t>
   </si>
   <si>
-    <t>Develop a Community Engagement Plan: Determine scope of engagement</t>
-  </si>
-  <si>
-    <t>Develop a Community Engagement Plan: Write the plan</t>
-  </si>
-  <si>
     <t>38</t>
   </si>
   <si>
-    <t>Reflection and next steps (Ch 2)</t>
-  </si>
-  <si>
     <t>39</t>
   </si>
   <si>
@@ -1193,9 +1139,6 @@
     <t>93</t>
   </si>
   <si>
-    <t>Plan Workshop While Centering Equity</t>
-  </si>
-  <si>
     <t>94</t>
   </si>
   <si>
@@ -1253,21 +1196,12 @@
     <t>106</t>
   </si>
   <si>
-    <t>Gather the Data</t>
-  </si>
-  <si>
     <t>107</t>
   </si>
   <si>
-    <t>Manage the Data</t>
-  </si>
-  <si>
     <t>108</t>
   </si>
   <si>
-    <t>Collaborate on Assessment</t>
-  </si>
-  <si>
     <t>109</t>
   </si>
   <si>
@@ -1286,24 +1220,15 @@
     <t>112</t>
   </si>
   <si>
-    <t>Reflection and Next Steps (Ch 3/4)</t>
-  </si>
-  <si>
     <t>Not in content.xml AND Not in contentXMLs directory</t>
   </si>
   <si>
     <t>Ch 3 About 4 column image</t>
   </si>
   <si>
-    <t>Ch 3 About 3 column image</t>
-  </si>
-  <si>
     <t>113</t>
   </si>
   <si>
-    <t>Ch 2 Activity 1 figure</t>
-  </si>
-  <si>
     <t>114</t>
   </si>
   <si>
@@ -1359,6 +1284,255 @@
   </si>
   <si>
     <t>Sorted Cards Example</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>Put Results into Action</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>Storytelling on Project Implementation</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>Workshop 3- Results to Action</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>Warm Up Activity</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>Create Vision Statements</t>
+  </si>
+  <si>
+    <t>Brainstorm Actions</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>Strategy Planning</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>Workshop Wrap-Up</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>Key Takeaways from Strategizing</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>Document Your Project</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>Use Monitoring to Support Future Action</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>Actions Brainstorming Example</t>
+  </si>
+  <si>
+    <t>(Section 1) Plan Your Project</t>
+  </si>
+  <si>
+    <t>Get a Core Team Together</t>
+  </si>
+  <si>
+    <t>Team Storytelling Exercise</t>
+  </si>
+  <si>
+    <t>Set Goals for Using ERB</t>
+  </si>
+  <si>
+    <t>Select ERB Activities</t>
+  </si>
+  <si>
+    <t>(Section 2) Engage Your Community</t>
+  </si>
+  <si>
+    <t>Identify Community Connections</t>
+  </si>
+  <si>
+    <t>Develop a Community Engagement Plan</t>
+  </si>
+  <si>
+    <t>Reflection and Next Steps (Ch 2)</t>
+  </si>
+  <si>
+    <t>Reflection and Next Steps (Ch 1)</t>
+  </si>
+  <si>
+    <t>(Section 3) Assess Hazards, Equity, and Resilience</t>
+  </si>
+  <si>
+    <t>Plan Workshop 1: Listen and Connect</t>
+  </si>
+  <si>
+    <t>Gather Data</t>
+  </si>
+  <si>
+    <t>Manage Data</t>
+  </si>
+  <si>
+    <t>Assess Resilience</t>
+  </si>
+  <si>
+    <t>Plan Workshop 2: Collaborative Assessment</t>
+  </si>
+  <si>
+    <t>Reflection and Next Steps (Ch 3)</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>Key Takeaways from Assessment</t>
+  </si>
+  <si>
+    <t>(Section 4) Strategize Actions</t>
+  </si>
+  <si>
+    <t>Define your Action Areas</t>
+  </si>
+  <si>
+    <t>Plan Workshop 3</t>
+  </si>
+  <si>
+    <t>Reflection and Next Steps (Ch 4)</t>
+  </si>
+  <si>
+    <t>(Section 5) Wrap Up and Move Forward</t>
+  </si>
+  <si>
+    <t>Implement Actions</t>
+  </si>
+  <si>
+    <t>Maintain Outreach and Engagement</t>
+  </si>
+  <si>
+    <t>Reflect and Celebrate (Ch 5)</t>
+  </si>
+  <si>
+    <t>Storytelling</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>Second Bullet</t>
+  </si>
+  <si>
+    <t>Equitable Resilience</t>
+  </si>
+  <si>
+    <t>The ERB Process</t>
+  </si>
+  <si>
+    <t>Trauma-informed Approach</t>
+  </si>
+  <si>
+    <t>Circle Picture. Trauma informed</t>
+  </si>
+  <si>
+    <t>Data Ethics</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>Types of data used in ERB</t>
+  </si>
+  <si>
+    <t>Resilience Indicators Background</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>Gather data on hazards, equity, and resilience</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>Youth Engagement. Figure 1.</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>Youth Engagement. Figure 2.</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Youth Engagement. Figure 3.</t>
+  </si>
+  <si>
+    <t>Youth Engagement Guide</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>Results to Action Workshop Agenda Builder</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>Strategy Chart Example</t>
+  </si>
+  <si>
+    <t>Strategy Chart Image</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>ERB Activity Chart</t>
   </si>
 </sst>
 </file>
@@ -1445,7 +1619,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1703,7 +1877,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1864,35 +2038,53 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1902,9 +2094,9 @@
   <colors>
     <mruColors>
       <color rgb="FFB1E36F"/>
+      <color rgb="FF80DEF8"/>
+      <color rgb="FFBAF8E2"/>
       <color rgb="FFFB9B9B"/>
-      <color rgb="FFBAF8E2"/>
-      <color rgb="FF80DEF8"/>
       <color rgb="FFE0C1FF"/>
     </mruColors>
   </colors>
@@ -2285,10 +2477,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="92" t="s">
+      <c r="G2" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="93"/>
+      <c r="H2" s="112"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5652,1420 +5844,2008 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="D151" sqref="D151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="96" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="90" customWidth="1"/>
     <col min="2" max="2" width="4" style="83" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="84" customWidth="1"/>
     <col min="4" max="4" width="80.85546875" style="84" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="66.7109375" style="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="87" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94"/>
-      <c r="B1" s="90" t="s">
+    <row r="1" spans="1:5" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="89"/>
+      <c r="B1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="88" t="s">
         <v>257</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="88" t="s">
         <v>256</v>
       </c>
-      <c r="E1" s="91" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="95"/>
-      <c r="B2" s="83" t="s">
+      <c r="E1" s="88" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="105"/>
+      <c r="B2" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="89" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="100" t="s">
+      <c r="C2" s="106" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="89"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="83" t="s">
+      <c r="E2" s="106"/>
+    </row>
+    <row r="3" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="92"/>
+      <c r="B3" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D3" s="85" t="s">
+      <c r="C3" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="94" t="s">
+        <v>470</v>
+      </c>
+      <c r="E3" s="94"/>
+    </row>
+    <row r="4" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="92"/>
+      <c r="B4" s="93" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>475</v>
+      </c>
+      <c r="E4" s="94"/>
+    </row>
+    <row r="5" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="92"/>
+      <c r="B5" s="93" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="94" t="s">
+        <v>473</v>
+      </c>
+      <c r="E5" s="94"/>
+    </row>
+    <row r="6" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="92"/>
+      <c r="B6" s="93" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="94" t="s">
+        <v>477</v>
+      </c>
+      <c r="E6" s="94"/>
+    </row>
+    <row r="7" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="92"/>
+      <c r="B7" s="93" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="94" t="s">
+        <v>480</v>
+      </c>
+      <c r="E7" s="94"/>
+    </row>
+    <row r="8" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="107"/>
+      <c r="B8" s="108" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="109" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="109" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D4" s="85" t="s">
+      <c r="E8" s="109"/>
+    </row>
+    <row r="9" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="107"/>
+      <c r="B9" s="108" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="83" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D5" s="85" t="s">
+      <c r="C9" s="109" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="109" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="83" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D6" s="85" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="83" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D7" s="85" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="83" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D8" s="85" t="s">
+      <c r="E9" s="109"/>
+    </row>
+    <row r="10" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="107"/>
+      <c r="B10" s="108" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="83" t="s">
+      <c r="C10" s="109" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="109" t="s">
         <v>263</v>
       </c>
-      <c r="C9" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" s="85" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="83" t="s">
-        <v>265</v>
-      </c>
-      <c r="C10" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="85" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="83" t="s">
+      <c r="E10" s="109"/>
+    </row>
+    <row r="11" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="92"/>
+      <c r="B11" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D11" s="85" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="83" t="s">
+      <c r="C11" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="94" t="s">
+        <v>489</v>
+      </c>
+      <c r="E11" s="94"/>
+    </row>
+    <row r="12" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="90"/>
+      <c r="B12" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D12" s="85" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="83" t="s">
+      <c r="E12" s="85"/>
+    </row>
+    <row r="13" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="90"/>
+      <c r="B13" s="91" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D13" s="85" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="83" t="s">
+      <c r="E13" s="85"/>
+    </row>
+    <row r="14" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="90"/>
+      <c r="B14" s="91" t="s">
         <v>159</v>
       </c>
-      <c r="C14" s="84" t="s">
+      <c r="C14" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D14" s="85" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="83" t="s">
+        <v>264</v>
+      </c>
+      <c r="E14" s="85"/>
+    </row>
+    <row r="15" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="90"/>
+      <c r="B15" s="91" t="s">
         <v>160</v>
       </c>
-      <c r="C15" s="84" t="s">
+      <c r="C15" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D15" s="85" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="83" t="s">
+      <c r="E15" s="85"/>
+    </row>
+    <row r="16" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="101"/>
+      <c r="B16" s="102" t="s">
+        <v>265</v>
+      </c>
+      <c r="C16" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D16" s="103" t="s">
+        <v>443</v>
+      </c>
+      <c r="E16" s="103"/>
+    </row>
+    <row r="17" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="101"/>
+      <c r="B17" s="102" t="s">
+        <v>266</v>
+      </c>
+      <c r="C17" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="103" t="s">
+        <v>448</v>
+      </c>
+      <c r="E17" s="103"/>
+    </row>
+    <row r="18" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="101"/>
+      <c r="B18" s="102" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="103" t="s">
+        <v>453</v>
+      </c>
+      <c r="E18" s="103"/>
+    </row>
+    <row r="19" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="101"/>
+      <c r="B19" s="102" t="s">
         <v>268</v>
       </c>
-      <c r="C16" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D16" s="85" t="s">
+      <c r="C19" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="103" t="s">
+        <v>462</v>
+      </c>
+      <c r="E19" s="103"/>
+    </row>
+    <row r="20" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="101"/>
+      <c r="B20" s="102" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="83" t="s">
+      <c r="C20" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="103" t="s">
+        <v>466</v>
+      </c>
+      <c r="E20" s="103"/>
+    </row>
+    <row r="21" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="101"/>
+      <c r="B21" s="102" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="103" t="s">
+        <v>445</v>
+      </c>
+      <c r="E21" s="103"/>
+    </row>
+    <row r="22" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="90"/>
+      <c r="B22" s="91" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" s="85" t="s">
         <v>270</v>
       </c>
-      <c r="C17" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D17" s="85" t="s">
+      <c r="E22" s="85"/>
+    </row>
+    <row r="23" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="90"/>
+      <c r="B23" s="91" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D23" s="85" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="83" t="s">
+      <c r="E23" s="85"/>
+    </row>
+    <row r="24" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="90"/>
+      <c r="B24" s="91" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D24" s="85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="85"/>
+    </row>
+    <row r="25" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="90"/>
+      <c r="B25" s="91" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" s="85" t="s">
         <v>272</v>
       </c>
-      <c r="C18" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="85" t="s">
+      <c r="D25" s="85" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="88"/>
-      <c r="B19" s="98" t="s">
+      <c r="E25" s="85"/>
+    </row>
+    <row r="26" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="101"/>
+      <c r="B26" s="102" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D26" s="103" t="s">
+        <v>464</v>
+      </c>
+      <c r="E26" s="103"/>
+    </row>
+    <row r="27" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="90"/>
+      <c r="B27" s="91" t="s">
         <v>274</v>
       </c>
-      <c r="C19" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D19" s="97" t="s">
+      <c r="C27" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D27" s="85" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
-      <c r="B20" s="98" t="s">
+      <c r="E27" s="85"/>
+    </row>
+    <row r="28" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="101"/>
+      <c r="B28" s="102" t="s">
         <v>276</v>
       </c>
-      <c r="C20" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="97" t="s">
+      <c r="C28" s="103" t="s">
+        <v>279</v>
+      </c>
+      <c r="D28" s="103" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="83" t="s">
-        <v>153</v>
-      </c>
-      <c r="C21" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D21" s="85" t="s">
+      <c r="E28" s="103"/>
+    </row>
+    <row r="29" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="101"/>
+      <c r="B29" s="102" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="88"/>
-      <c r="B22" s="98" t="s">
-        <v>161</v>
-      </c>
-      <c r="C22" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D22" s="97" t="s">
+      <c r="C29" s="103" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="88"/>
-      <c r="B23" s="98" t="s">
-        <v>162</v>
-      </c>
-      <c r="C23" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D23" s="97" t="s">
+      <c r="D29" s="103" t="s">
+        <v>233</v>
+      </c>
+      <c r="E29" s="103"/>
+    </row>
+    <row r="30" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="101"/>
+      <c r="B30" s="102" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="88"/>
-      <c r="B24" s="98" t="s">
-        <v>163</v>
-      </c>
-      <c r="C24" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D24" s="97" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="88"/>
-      <c r="B25" s="98" t="s">
-        <v>164</v>
-      </c>
-      <c r="C25" s="97" t="s">
+      <c r="C30" s="103" t="s">
+        <v>279</v>
+      </c>
+      <c r="D30" s="103" t="s">
+        <v>234</v>
+      </c>
+      <c r="E30" s="103"/>
+    </row>
+    <row r="31" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="101"/>
+      <c r="B31" s="102" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="103" t="s">
+        <v>444</v>
+      </c>
+      <c r="E31" s="103"/>
+    </row>
+    <row r="32" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="101"/>
+      <c r="B32" s="102" t="s">
+        <v>166</v>
+      </c>
+      <c r="C32" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D32" s="103" t="s">
+        <v>447</v>
+      </c>
+      <c r="E32" s="103"/>
+    </row>
+    <row r="33" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="101"/>
+      <c r="B33" s="102" t="s">
+        <v>167</v>
+      </c>
+      <c r="C33" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D33" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="103"/>
+    </row>
+    <row r="34" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="101"/>
+      <c r="B34" s="102" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="103" t="s">
+        <v>452</v>
+      </c>
+      <c r="E34" s="103"/>
+    </row>
+    <row r="35" spans="1:5" s="104" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="101"/>
+      <c r="B35" s="102" t="s">
+        <v>169</v>
+      </c>
+      <c r="C35" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D35" s="103" t="s">
+        <v>449</v>
+      </c>
+      <c r="E35" s="103"/>
+    </row>
+    <row r="36" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="101"/>
+      <c r="B36" s="102" t="s">
+        <v>170</v>
+      </c>
+      <c r="C36" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D36" s="103" t="s">
         <v>281</v>
       </c>
-      <c r="D25" s="97" t="s">
+      <c r="E36" s="103"/>
+    </row>
+    <row r="37" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="101"/>
+      <c r="B37" s="102" t="s">
+        <v>171</v>
+      </c>
+      <c r="C37" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" s="103" t="s">
+        <v>450</v>
+      </c>
+      <c r="E37" s="103"/>
+    </row>
+    <row r="38" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="101"/>
+      <c r="B38" s="102" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D38" s="103" t="s">
+        <v>458</v>
+      </c>
+      <c r="E38" s="103"/>
+    </row>
+    <row r="39" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="101"/>
+      <c r="B39" s="102" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="88"/>
-      <c r="B26" s="98" t="s">
-        <v>165</v>
-      </c>
-      <c r="C26" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D26" s="97" t="s">
+      <c r="C39" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" s="103" t="s">
+        <v>451</v>
+      </c>
+      <c r="E39" s="103"/>
+    </row>
+    <row r="40" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="90"/>
+      <c r="B40" s="91" t="s">
+        <v>283</v>
+      </c>
+      <c r="C40" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D40" s="85" t="s">
+        <v>284</v>
+      </c>
+      <c r="E40" s="85"/>
+    </row>
+    <row r="41" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="90"/>
+      <c r="B41" s="91" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D41" s="85" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="88"/>
-      <c r="B27" s="98" t="s">
-        <v>283</v>
-      </c>
-      <c r="C27" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D27" s="97" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="83" t="s">
+      <c r="E41" s="85"/>
+    </row>
+    <row r="42" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="90"/>
+      <c r="B42" s="91" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D42" s="85" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="85"/>
+    </row>
+    <row r="43" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="90"/>
+      <c r="B43" s="91" t="s">
+        <v>175</v>
+      </c>
+      <c r="C43" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D43" s="85" t="s">
         <v>286</v>
       </c>
-      <c r="C28" s="84" t="s">
+      <c r="E43" s="85"/>
+    </row>
+    <row r="44" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="90"/>
+      <c r="B44" s="91" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D44" s="85" t="s">
+        <v>287</v>
+      </c>
+      <c r="E44" s="85"/>
+    </row>
+    <row r="45" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="90"/>
+      <c r="B45" s="91" t="s">
+        <v>177</v>
+      </c>
+      <c r="C45" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="85" t="s">
+        <v>288</v>
+      </c>
+      <c r="E45" s="85"/>
+    </row>
+    <row r="46" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="90"/>
+      <c r="B46" s="91" t="s">
         <v>289</v>
       </c>
-      <c r="D28" s="85" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="83" t="s">
-        <v>288</v>
-      </c>
-      <c r="C29" s="84" t="s">
-        <v>289</v>
-      </c>
-      <c r="D29" s="85" t="s">
+      <c r="C46" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D46" s="85" t="s">
+        <v>290</v>
+      </c>
+      <c r="E46" s="85"/>
+    </row>
+    <row r="47" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="90"/>
+      <c r="B47" s="91" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="83" t="s">
-        <v>290</v>
-      </c>
-      <c r="C30" s="84" t="s">
-        <v>289</v>
-      </c>
-      <c r="D30" s="85" t="s">
+      <c r="C47" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="85" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="83" t="s">
-        <v>154</v>
-      </c>
-      <c r="C31" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D31" s="85" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="99" t="s">
-        <v>166</v>
-      </c>
-      <c r="C32" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D32" s="85" t="s">
+      <c r="E47" s="85"/>
+    </row>
+    <row r="48" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="90"/>
+      <c r="B48" s="91" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="83" t="s">
-        <v>167</v>
-      </c>
-      <c r="C33" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D33" s="85" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="83" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D34" s="85" t="s">
+      <c r="C48" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" s="85" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="85"/>
+    </row>
+    <row r="49" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="90"/>
+      <c r="B49" s="91" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="83" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D35" s="85" t="s">
+      <c r="C49" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D49" s="85" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="85"/>
+    </row>
+    <row r="50" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="90"/>
+      <c r="B50" s="91" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="83" t="s">
-        <v>170</v>
-      </c>
-      <c r="C36" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D36" s="85" t="s">
+      <c r="C50" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" s="85" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="83" t="s">
-        <v>171</v>
-      </c>
-      <c r="C37" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D37" s="85" t="s">
+      <c r="E50" s="85"/>
+    </row>
+    <row r="51" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="90"/>
+      <c r="B51" s="91" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" s="85" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="85"/>
+    </row>
+    <row r="52" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="90"/>
+      <c r="B52" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D52" s="85" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="85"/>
+    </row>
+    <row r="53" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="90"/>
+      <c r="B53" s="91" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D53" s="85" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="83" t="s">
-        <v>172</v>
-      </c>
-      <c r="C38" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D38" s="85" t="s">
+      <c r="E53" s="85"/>
+    </row>
+    <row r="54" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="90"/>
+      <c r="B54" s="91" t="s">
+        <v>180</v>
+      </c>
+      <c r="C54" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D54" s="85" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" s="85"/>
+    </row>
+    <row r="55" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="90"/>
+      <c r="B55" s="91" t="s">
+        <v>181</v>
+      </c>
+      <c r="C55" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D55" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55" s="85"/>
+    </row>
+    <row r="56" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="90"/>
+      <c r="B56" s="91" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D56" s="85" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="83" t="s">
+      <c r="E56" s="85"/>
+    </row>
+    <row r="57" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="90"/>
+      <c r="B57" s="91" t="s">
+        <v>183</v>
+      </c>
+      <c r="C57" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D57" s="85" t="s">
         <v>299</v>
       </c>
-      <c r="C39" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D39" s="85" t="s">
+      <c r="E57" s="85"/>
+    </row>
+    <row r="58" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="90"/>
+      <c r="B58" s="91" t="s">
+        <v>184</v>
+      </c>
+      <c r="C58" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D58" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="85"/>
+    </row>
+    <row r="59" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="90"/>
+      <c r="B59" s="91" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D59" s="85" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="88"/>
-      <c r="B40" s="98" t="s">
+      <c r="E59" s="85"/>
+    </row>
+    <row r="60" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="101"/>
+      <c r="B60" s="102" t="s">
+        <v>186</v>
+      </c>
+      <c r="C60" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="103" t="s">
+        <v>446</v>
+      </c>
+      <c r="E60" s="103"/>
+    </row>
+    <row r="61" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="101"/>
+      <c r="B61" s="102" t="s">
         <v>301</v>
       </c>
-      <c r="C40" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D40" s="97" t="s">
+      <c r="C61" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D61" s="103" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="88"/>
-      <c r="B41" s="98" t="s">
-        <v>155</v>
-      </c>
-      <c r="C41" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D41" s="97" t="s">
+      <c r="E61" s="103"/>
+    </row>
+    <row r="62" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="101"/>
+      <c r="B62" s="102" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="88"/>
-      <c r="B42" s="98" t="s">
-        <v>174</v>
-      </c>
-      <c r="C42" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D42" s="97" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="88"/>
-      <c r="B43" s="98" t="s">
-        <v>175</v>
-      </c>
-      <c r="C43" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D43" s="97" t="s">
+      <c r="C62" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D62" s="103" t="s">
+        <v>230</v>
+      </c>
+      <c r="E62" s="103"/>
+    </row>
+    <row r="63" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="101"/>
+      <c r="B63" s="102" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="88"/>
-      <c r="B44" s="98" t="s">
-        <v>176</v>
-      </c>
-      <c r="C44" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D44" s="97" t="s">
+      <c r="C63" s="103" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="88"/>
-      <c r="B45" s="98" t="s">
-        <v>177</v>
-      </c>
-      <c r="C45" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D45" s="97" t="s">
+      <c r="D63" s="103" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="88"/>
-      <c r="B46" s="98" t="s">
+      <c r="E63" s="103"/>
+    </row>
+    <row r="64" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="101"/>
+      <c r="B64" s="102" t="s">
         <v>307</v>
       </c>
-      <c r="C46" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D46" s="97" t="s">
+      <c r="C64" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D64" s="103" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="88"/>
-      <c r="B47" s="98" t="s">
+      <c r="E64" s="103"/>
+    </row>
+    <row r="65" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="101"/>
+      <c r="B65" s="102" t="s">
         <v>309</v>
       </c>
-      <c r="C47" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D47" s="97" t="s">
+      <c r="C65" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D65" s="103" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="88"/>
-      <c r="B48" s="98" t="s">
+      <c r="E65" s="103"/>
+    </row>
+    <row r="66" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="101"/>
+      <c r="B66" s="102" t="s">
         <v>311</v>
       </c>
-      <c r="C48" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D48" s="97" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="88"/>
-      <c r="B49" s="98" t="s">
+      <c r="C66" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D66" s="103" t="s">
         <v>312</v>
       </c>
-      <c r="C49" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D49" s="97" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="88"/>
-      <c r="B50" s="98" t="s">
+      <c r="E66" s="103"/>
+    </row>
+    <row r="67" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="101"/>
+      <c r="B67" s="102" t="s">
         <v>313</v>
       </c>
-      <c r="C50" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D50" s="97" t="s">
+      <c r="C67" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D67" s="103" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="88"/>
-      <c r="B51" s="98" t="s">
-        <v>156</v>
-      </c>
-      <c r="C51" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D51" s="97" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="88"/>
-      <c r="B52" s="98" t="s">
-        <v>178</v>
-      </c>
-      <c r="C52" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" s="97" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="88"/>
-      <c r="B53" s="98" t="s">
-        <v>179</v>
-      </c>
-      <c r="C53" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D53" s="97" t="s">
+      <c r="E67" s="103"/>
+    </row>
+    <row r="68" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="101"/>
+      <c r="B68" s="102" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="88"/>
-      <c r="B54" s="98" t="s">
-        <v>180</v>
-      </c>
-      <c r="C54" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D54" s="97" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="88"/>
-      <c r="B55" s="98" t="s">
-        <v>181</v>
-      </c>
-      <c r="C55" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D55" s="97" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="88"/>
-      <c r="B56" s="98" t="s">
-        <v>182</v>
-      </c>
-      <c r="C56" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D56" s="97" t="s">
+      <c r="C68" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D68" s="103" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="88"/>
-      <c r="B57" s="98" t="s">
-        <v>183</v>
-      </c>
-      <c r="C57" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D57" s="97" t="s">
+      <c r="E68" s="103"/>
+    </row>
+    <row r="69" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="101"/>
+      <c r="B69" s="102" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="88"/>
-      <c r="B58" s="98" t="s">
-        <v>184</v>
-      </c>
-      <c r="C58" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D58" s="97" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="88"/>
-      <c r="B59" s="98" t="s">
-        <v>185</v>
-      </c>
-      <c r="C59" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D59" s="97" t="s">
+      <c r="C69" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D69" s="103" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="83" t="s">
-        <v>186</v>
-      </c>
-      <c r="C60" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D60" s="85" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="83" t="s">
+      <c r="E69" s="103"/>
+    </row>
+    <row r="70" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="101"/>
+      <c r="B70" s="102" t="s">
         <v>319</v>
       </c>
-      <c r="C61" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D61" s="85" t="s">
+      <c r="C70" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D70" s="103" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="83" t="s">
+      <c r="E70" s="103"/>
+    </row>
+    <row r="71" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="101"/>
+      <c r="B71" s="102" t="s">
         <v>321</v>
       </c>
-      <c r="C62" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D62" s="85" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="83" t="s">
+      <c r="C71" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D71" s="103" t="s">
         <v>322</v>
       </c>
-      <c r="C63" s="84" t="s">
+      <c r="E71" s="103"/>
+    </row>
+    <row r="72" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="101"/>
+      <c r="B72" s="102" t="s">
         <v>323</v>
       </c>
-      <c r="D63" s="84" t="s">
+      <c r="C72" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D72" s="103" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="83" t="s">
+      <c r="E72" s="103"/>
+    </row>
+    <row r="73" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="101"/>
+      <c r="B73" s="102" t="s">
         <v>325</v>
       </c>
-      <c r="C64" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D64" s="84" t="s">
+      <c r="C73" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D73" s="103" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="83" t="s">
+      <c r="E73" s="103"/>
+    </row>
+    <row r="74" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="101"/>
+      <c r="B74" s="102" t="s">
         <v>327</v>
       </c>
-      <c r="C65" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D65" s="84" t="s">
+      <c r="C74" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D74" s="103" t="s">
+        <v>221</v>
+      </c>
+      <c r="E74" s="103"/>
+    </row>
+    <row r="75" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="101"/>
+      <c r="B75" s="102" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="83" t="s">
+      <c r="C75" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D75" s="103" t="s">
         <v>329</v>
       </c>
-      <c r="C66" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D66" s="84" t="s">
+      <c r="E75" s="103"/>
+    </row>
+    <row r="76" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="101"/>
+      <c r="B76" s="102" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="83" t="s">
+      <c r="C76" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D76" s="103" t="s">
         <v>331</v>
       </c>
-      <c r="C67" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D67" s="84" t="s">
+      <c r="E76" s="103"/>
+    </row>
+    <row r="77" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="101"/>
+      <c r="B77" s="102" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="83" t="s">
+      <c r="C77" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D77" s="103" t="s">
         <v>333</v>
       </c>
-      <c r="C68" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D68" s="84" t="s">
+      <c r="E77" s="103"/>
+    </row>
+    <row r="78" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="101"/>
+      <c r="B78" s="102" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="83" t="s">
+      <c r="C78" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D78" s="103" t="s">
         <v>335</v>
       </c>
-      <c r="C69" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D69" s="84" t="s">
+      <c r="E78" s="103"/>
+    </row>
+    <row r="79" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="101"/>
+      <c r="B79" s="102" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="83" t="s">
+      <c r="C79" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D79" s="103" t="s">
         <v>337</v>
       </c>
-      <c r="C70" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D70" s="84" t="s">
+      <c r="E79" s="103"/>
+    </row>
+    <row r="80" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="101"/>
+      <c r="B80" s="102" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="83" t="s">
+      <c r="C80" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="C71" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D71" s="84" t="s">
+      <c r="D80" s="103" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="83" t="s">
+      <c r="E80" s="103"/>
+    </row>
+    <row r="81" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="101"/>
+      <c r="B81" s="102" t="s">
         <v>341</v>
       </c>
-      <c r="C72" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D72" s="84" t="s">
+      <c r="C81" s="103" t="s">
+        <v>339</v>
+      </c>
+      <c r="D81" s="103" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="83" t="s">
+      <c r="E81" s="103"/>
+    </row>
+    <row r="82" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="101"/>
+      <c r="B82" s="102" t="s">
         <v>343</v>
       </c>
-      <c r="C73" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D73" s="84" t="s">
+      <c r="C82" s="103" t="s">
+        <v>339</v>
+      </c>
+      <c r="D82" s="103" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="83" t="s">
+      <c r="E82" s="103"/>
+    </row>
+    <row r="83" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="101"/>
+      <c r="B83" s="102" t="s">
         <v>345</v>
       </c>
-      <c r="C74" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D74" s="84" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="83" t="s">
+      <c r="C83" s="103" t="s">
+        <v>339</v>
+      </c>
+      <c r="D83" s="103" t="s">
+        <v>233</v>
+      </c>
+      <c r="E83" s="103"/>
+    </row>
+    <row r="84" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="101"/>
+      <c r="B84" s="102" t="s">
         <v>346</v>
       </c>
-      <c r="C75" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D75" s="84" t="s">
+      <c r="C84" s="103" t="s">
+        <v>339</v>
+      </c>
+      <c r="D84" s="103" t="s">
+        <v>234</v>
+      </c>
+      <c r="E84" s="103"/>
+    </row>
+    <row r="85" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="101"/>
+      <c r="B85" s="102" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="83" t="s">
+      <c r="C85" s="103" t="s">
         <v>348</v>
       </c>
-      <c r="C76" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D76" s="84" t="s">
+      <c r="D85" s="103" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="83" t="s">
+      <c r="E85" s="103" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="101"/>
+      <c r="B86" s="102" t="s">
         <v>350</v>
       </c>
-      <c r="C77" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D77" s="84" t="s">
+      <c r="C86" s="103" t="s">
+        <v>348</v>
+      </c>
+      <c r="D86" s="103" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="83" t="s">
+      <c r="E86" s="103" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="90"/>
+      <c r="B87" s="91" t="s">
+        <v>353</v>
+      </c>
+      <c r="C87" s="85" t="s">
         <v>352</v>
-      </c>
-      <c r="C78" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D78" s="84" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="83" t="s">
-        <v>354</v>
-      </c>
-      <c r="C79" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D79" s="84" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="83" t="s">
-        <v>356</v>
-      </c>
-      <c r="C80" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D80" s="84" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="83" t="s">
-        <v>359</v>
-      </c>
-      <c r="C81" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D81" s="84" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="83" t="s">
-        <v>361</v>
-      </c>
-      <c r="C82" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D82" s="84" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="83" t="s">
-        <v>363</v>
-      </c>
-      <c r="C83" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D83" s="84" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="83" t="s">
-        <v>364</v>
-      </c>
-      <c r="C84" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D84" s="85" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="83" t="s">
-        <v>365</v>
-      </c>
-      <c r="C85" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="D85" s="85" t="s">
-        <v>367</v>
-      </c>
-      <c r="E85" s="84" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="83" t="s">
-        <v>368</v>
-      </c>
-      <c r="C86" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="D86" s="85" t="s">
-        <v>369</v>
-      </c>
-      <c r="E86" s="84" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="83" t="s">
-        <v>371</v>
-      </c>
-      <c r="C87" s="84" t="s">
-        <v>370</v>
       </c>
       <c r="D87" s="85" t="s">
         <v>193</v>
       </c>
-      <c r="E87" s="86" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="83" t="s">
-        <v>372</v>
-      </c>
-      <c r="C88" s="84" t="s">
-        <v>370</v>
+      <c r="E87" s="97" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="90"/>
+      <c r="B88" s="91" t="s">
+        <v>354</v>
+      </c>
+      <c r="C88" s="85" t="s">
+        <v>352</v>
       </c>
       <c r="D88" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="E88" s="86" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="83" t="s">
-        <v>373</v>
-      </c>
-      <c r="C89" s="84" t="s">
-        <v>370</v>
+      <c r="E88" s="97" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="90"/>
+      <c r="B89" s="91" t="s">
+        <v>355</v>
+      </c>
+      <c r="C89" s="85" t="s">
+        <v>352</v>
       </c>
       <c r="D89" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="E89" s="86" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="83" t="s">
-        <v>374</v>
-      </c>
-      <c r="C90" s="84" t="s">
-        <v>370</v>
+      <c r="E89" s="97" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="90"/>
+      <c r="B90" s="91" t="s">
+        <v>356</v>
+      </c>
+      <c r="C90" s="85" t="s">
+        <v>352</v>
       </c>
       <c r="D90" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="E90" s="86" t="s">
+      <c r="E90" s="97" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="90"/>
+      <c r="B91" s="91" t="s">
+        <v>357</v>
+      </c>
+      <c r="C91" s="85" t="s">
+        <v>352</v>
+      </c>
+      <c r="D91" s="85" t="s">
+        <v>358</v>
+      </c>
+      <c r="E91" s="97" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="90"/>
+      <c r="B92" s="91" t="s">
+        <v>360</v>
+      </c>
+      <c r="C92" s="85" t="s">
+        <v>352</v>
+      </c>
+      <c r="D92" s="85" t="s">
+        <v>361</v>
+      </c>
+      <c r="E92" s="97" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="101"/>
+      <c r="B93" s="102" t="s">
+        <v>363</v>
+      </c>
+      <c r="C93" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D93" s="103" t="s">
+        <v>364</v>
+      </c>
+      <c r="E93" s="103"/>
+    </row>
+    <row r="94" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="101"/>
+      <c r="B94" s="102" t="s">
+        <v>365</v>
+      </c>
+      <c r="C94" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="103" t="s">
+        <v>454</v>
+      </c>
+      <c r="E94" s="103"/>
+    </row>
+    <row r="95" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="101"/>
+      <c r="B95" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="C95" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="103" t="s">
+        <v>367</v>
+      </c>
+      <c r="E95" s="103"/>
+    </row>
+    <row r="96" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="101"/>
+      <c r="B96" s="102" t="s">
+        <v>368</v>
+      </c>
+      <c r="C96" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D96" s="103" t="s">
+        <v>369</v>
+      </c>
+      <c r="E96" s="103"/>
+    </row>
+    <row r="97" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="101"/>
+      <c r="B97" s="102" t="s">
+        <v>370</v>
+      </c>
+      <c r="C97" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D97" s="103" t="s">
+        <v>371</v>
+      </c>
+      <c r="E97" s="103"/>
+    </row>
+    <row r="98" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="101"/>
+      <c r="B98" s="102" t="s">
+        <v>372</v>
+      </c>
+      <c r="C98" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" s="103" t="s">
+        <v>373</v>
+      </c>
+      <c r="E98" s="103"/>
+    </row>
+    <row r="99" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="101"/>
+      <c r="B99" s="102" t="s">
+        <v>374</v>
+      </c>
+      <c r="C99" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D99" s="103" t="s">
+        <v>375</v>
+      </c>
+      <c r="E99" s="103"/>
+    </row>
+    <row r="100" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="101"/>
+      <c r="B100" s="102" t="s">
+        <v>378</v>
+      </c>
+      <c r="C100" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" s="103" t="s">
+        <v>379</v>
+      </c>
+      <c r="E100" s="103"/>
+    </row>
+    <row r="101" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="101"/>
+      <c r="B101" s="102" t="s">
+        <v>380</v>
+      </c>
+      <c r="C101" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" s="103" t="s">
+        <v>381</v>
+      </c>
+      <c r="E101" s="103"/>
+    </row>
+    <row r="102" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="101"/>
+      <c r="B102" s="102" t="s">
+        <v>382</v>
+      </c>
+      <c r="C102" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D102" s="103" t="s">
+        <v>383</v>
+      </c>
+      <c r="E102" s="103"/>
+    </row>
+    <row r="103" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="101"/>
+      <c r="B103" s="102" t="s">
+        <v>384</v>
+      </c>
+      <c r="C103" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" s="103" t="s">
+        <v>455</v>
+      </c>
+      <c r="E103" s="103"/>
+    </row>
+    <row r="104" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="101"/>
+      <c r="B104" s="102" t="s">
+        <v>385</v>
+      </c>
+      <c r="C104" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D104" s="103" t="s">
+        <v>456</v>
+      </c>
+      <c r="E104" s="103"/>
+    </row>
+    <row r="105" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="101"/>
+      <c r="B105" s="102" t="s">
+        <v>386</v>
+      </c>
+      <c r="C105" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="103" t="s">
+        <v>457</v>
+      </c>
+      <c r="E105" s="103"/>
+    </row>
+    <row r="106" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="101"/>
+      <c r="B106" s="102" t="s">
+        <v>387</v>
+      </c>
+      <c r="C106" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D106" s="103" t="s">
+        <v>388</v>
+      </c>
+      <c r="E106" s="103"/>
+    </row>
+    <row r="107" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="101"/>
+      <c r="B107" s="102" t="s">
+        <v>389</v>
+      </c>
+      <c r="C107" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D107" s="103" t="s">
+        <v>390</v>
+      </c>
+      <c r="E107" s="103"/>
+    </row>
+    <row r="108" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="101"/>
+      <c r="B108" s="102" t="s">
+        <v>187</v>
+      </c>
+      <c r="C108" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D108" s="103" t="s">
+        <v>391</v>
+      </c>
+      <c r="E108" s="103"/>
+    </row>
+    <row r="109" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="101"/>
+      <c r="B109" s="102" t="s">
+        <v>392</v>
+      </c>
+      <c r="C109" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D109" s="103" t="s">
+        <v>459</v>
+      </c>
+      <c r="E109" s="103"/>
+    </row>
+    <row r="110" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="90"/>
+      <c r="B110" s="91" t="s">
+        <v>376</v>
+      </c>
+      <c r="C110" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D110" s="85" t="s">
+        <v>394</v>
+      </c>
+      <c r="E110" s="85"/>
+    </row>
+    <row r="111" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="90"/>
+      <c r="B111" s="91" t="s">
+        <v>377</v>
+      </c>
+      <c r="C111" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D111" s="85" t="s">
+        <v>474</v>
+      </c>
+      <c r="E111" s="85"/>
+    </row>
+    <row r="112" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="90"/>
+      <c r="B112" s="91" t="s">
+        <v>395</v>
+      </c>
+      <c r="C112" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D112" s="85" t="s">
+        <v>476</v>
+      </c>
+      <c r="E112" s="85"/>
+    </row>
+    <row r="113" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="101"/>
+      <c r="B113" s="102" t="s">
+        <v>396</v>
+      </c>
+      <c r="C113" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D113" s="103" t="s">
+        <v>397</v>
+      </c>
+      <c r="E113" s="103"/>
+    </row>
+    <row r="114" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="101"/>
+      <c r="B114" s="102" t="s">
+        <v>398</v>
+      </c>
+      <c r="C114" s="103" t="s">
+        <v>339</v>
+      </c>
+      <c r="D114" s="103" t="s">
+        <v>399</v>
+      </c>
+      <c r="E114" s="103"/>
+    </row>
+    <row r="115" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="101"/>
+      <c r="B115" s="102" t="s">
+        <v>400</v>
+      </c>
+      <c r="C115" s="103" t="s">
+        <v>279</v>
+      </c>
+      <c r="D115" s="103" t="s">
+        <v>401</v>
+      </c>
+      <c r="E115" s="103"/>
+    </row>
+    <row r="116" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="90"/>
+      <c r="B116" s="91" t="s">
+        <v>402</v>
+      </c>
+      <c r="C116" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D116" s="85" t="s">
+        <v>403</v>
+      </c>
+      <c r="E116" s="85"/>
+    </row>
+    <row r="117" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="101"/>
+      <c r="B117" s="102" t="s">
+        <v>404</v>
+      </c>
+      <c r="C117" s="103" t="s">
+        <v>279</v>
+      </c>
+      <c r="D117" s="103" t="s">
+        <v>405</v>
+      </c>
+      <c r="E117" s="103"/>
+    </row>
+    <row r="118" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="90"/>
+      <c r="B118" s="91" t="s">
+        <v>406</v>
+      </c>
+      <c r="C118" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D118" s="85" t="s">
+        <v>407</v>
+      </c>
+      <c r="E118" s="85"/>
+    </row>
+    <row r="119" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="101"/>
+      <c r="B119" s="102" t="s">
+        <v>408</v>
+      </c>
+      <c r="C119" s="103" t="s">
+        <v>339</v>
+      </c>
+      <c r="D119" s="103" t="s">
+        <v>409</v>
+      </c>
+      <c r="E119" s="103"/>
+    </row>
+    <row r="120" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="101"/>
+      <c r="B120" s="102" t="s">
+        <v>188</v>
+      </c>
+      <c r="C120" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D120" s="103" t="s">
+        <v>410</v>
+      </c>
+      <c r="E120" s="103"/>
+    </row>
+    <row r="121" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="101"/>
+      <c r="B121" s="102" t="s">
+        <v>411</v>
+      </c>
+      <c r="C121" s="103" t="s">
+        <v>339</v>
+      </c>
+      <c r="D121" s="103" t="s">
+        <v>413</v>
+      </c>
+      <c r="E121" s="103"/>
+    </row>
+    <row r="122" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="101"/>
+      <c r="B122" s="102" t="s">
+        <v>412</v>
+      </c>
+      <c r="C122" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D122" s="103" t="s">
+        <v>414</v>
+      </c>
+      <c r="E122" s="103"/>
+    </row>
+    <row r="123" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="101"/>
+      <c r="B123" s="102" t="s">
+        <v>415</v>
+      </c>
+      <c r="C123" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D123" s="103" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="83" t="s">
-        <v>375</v>
-      </c>
-      <c r="C91" s="84" t="s">
-        <v>370</v>
-      </c>
-      <c r="D91" s="85" t="s">
-        <v>376</v>
-      </c>
-      <c r="E91" s="86" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="83" t="s">
-        <v>378</v>
-      </c>
-      <c r="C92" s="84" t="s">
-        <v>370</v>
-      </c>
-      <c r="D92" s="85" t="s">
-        <v>379</v>
-      </c>
-      <c r="E92" s="86" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="83" t="s">
-        <v>381</v>
-      </c>
-      <c r="C93" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D93" s="85" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="83" t="s">
-        <v>383</v>
-      </c>
-      <c r="C94" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D94" s="85" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="83" t="s">
-        <v>385</v>
-      </c>
-      <c r="C95" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D95" s="85" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="83" t="s">
-        <v>387</v>
-      </c>
-      <c r="C96" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D96" s="85" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="83" t="s">
-        <v>389</v>
-      </c>
-      <c r="C97" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D97" s="85" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="83" t="s">
-        <v>391</v>
-      </c>
-      <c r="C98" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D98" s="85" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="83" t="s">
-        <v>393</v>
-      </c>
-      <c r="C99" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D99" s="85" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="83" t="s">
-        <v>397</v>
-      </c>
-      <c r="C100" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D100" s="85" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="83" t="s">
-        <v>399</v>
-      </c>
-      <c r="C101" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D101" s="85" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="83" t="s">
-        <v>401</v>
-      </c>
-      <c r="C102" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D102" s="85" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="83" t="s">
-        <v>403</v>
-      </c>
-      <c r="C103" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D103" s="85" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="83" t="s">
-        <v>405</v>
-      </c>
-      <c r="C104" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D104" s="85" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="83" t="s">
-        <v>407</v>
-      </c>
-      <c r="C105" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D105" s="85" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="83" t="s">
-        <v>409</v>
-      </c>
-      <c r="C106" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D106" s="85" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="83" t="s">
-        <v>411</v>
-      </c>
-      <c r="C107" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D107" s="85" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="83" t="s">
-        <v>187</v>
-      </c>
-      <c r="C108" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D108" s="85" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="83" t="s">
-        <v>414</v>
-      </c>
-      <c r="C109" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D109" s="85" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="83" t="s">
-        <v>395</v>
-      </c>
-      <c r="C110" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D110" s="84" t="s">
+      <c r="E123" s="103"/>
+    </row>
+    <row r="124" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="101"/>
+      <c r="B124" s="102" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="83" t="s">
-        <v>396</v>
-      </c>
-      <c r="C111" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D111" s="84" t="s">
+      <c r="C124" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D124" s="103" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="83" t="s">
+      <c r="E124" s="103"/>
+    </row>
+    <row r="125" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="101"/>
+      <c r="B125" s="102" t="s">
         <v>419</v>
       </c>
-      <c r="C112" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D112" s="84" t="s">
+      <c r="C125" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D125" s="103" t="s">
+        <v>463</v>
+      </c>
+      <c r="E125" s="103"/>
+    </row>
+    <row r="126" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="101"/>
+      <c r="B126" s="102" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="83" t="s">
+      <c r="C126" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D126" s="103" t="s">
         <v>421</v>
       </c>
-      <c r="C113" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D113" s="84" t="s">
+      <c r="E126" s="103"/>
+    </row>
+    <row r="127" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="101"/>
+      <c r="B127" s="102" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="83" t="s">
+      <c r="C127" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D127" s="103" t="s">
         <v>423</v>
       </c>
-      <c r="C114" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D114" s="84" t="s">
+      <c r="E127" s="103"/>
+    </row>
+    <row r="128" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="101"/>
+      <c r="B128" s="102" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="83" t="s">
+      <c r="C128" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D128" s="103" t="s">
         <v>425</v>
       </c>
-      <c r="C115" s="84" t="s">
-        <v>289</v>
-      </c>
-      <c r="D115" s="84" t="s">
+      <c r="E128" s="103"/>
+    </row>
+    <row r="129" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="101"/>
+      <c r="B129" s="102" t="s">
+        <v>189</v>
+      </c>
+      <c r="C129" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D129" s="103" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="83" t="s">
+      <c r="E129" s="103"/>
+    </row>
+    <row r="130" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="101"/>
+      <c r="B130" s="102" t="s">
+        <v>190</v>
+      </c>
+      <c r="C130" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D130" s="103" t="s">
+        <v>298</v>
+      </c>
+      <c r="E130" s="103"/>
+    </row>
+    <row r="131" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="101"/>
+      <c r="B131" s="102" t="s">
         <v>427</v>
       </c>
-      <c r="C116" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D116" s="84" t="s">
+      <c r="C131" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D131" s="103" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="83" t="s">
+      <c r="E131" s="103"/>
+    </row>
+    <row r="132" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="101"/>
+      <c r="B132" s="102" t="s">
         <v>429</v>
       </c>
-      <c r="C117" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D117" s="84" t="s">
+      <c r="C132" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D132" s="103" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="83" t="s">
+      <c r="E132" s="103"/>
+    </row>
+    <row r="133" spans="1:5" s="104" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="101"/>
+      <c r="B133" s="102" t="s">
         <v>431</v>
       </c>
-      <c r="C118" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D118" s="84" t="s">
+      <c r="C133" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D133" s="103" t="s">
+        <v>465</v>
+      </c>
+      <c r="E133" s="103"/>
+    </row>
+    <row r="134" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="101"/>
+      <c r="B134" s="102" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="83" t="s">
+      <c r="C134" s="103" t="s">
+        <v>272</v>
+      </c>
+      <c r="D134" s="103" t="s">
         <v>433</v>
       </c>
-      <c r="C119" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D119" s="84" t="s">
+      <c r="E134" s="103"/>
+    </row>
+    <row r="135" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="101"/>
+      <c r="B135" s="102" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="83" t="s">
-        <v>188</v>
-      </c>
-      <c r="C120" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D120" s="84" t="s">
+      <c r="C135" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D135" s="103" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="83" t="s">
+      <c r="E135" s="103"/>
+    </row>
+    <row r="136" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="101"/>
+      <c r="B136" s="102" t="s">
         <v>436</v>
       </c>
-      <c r="C121" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D121" s="84" t="s">
+      <c r="C136" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D136" s="103" t="s">
+        <v>468</v>
+      </c>
+      <c r="E136" s="103"/>
+    </row>
+    <row r="137" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="101"/>
+      <c r="B137" s="102" t="s">
+        <v>437</v>
+      </c>
+      <c r="C137" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D137" s="103" t="s">
+        <v>467</v>
+      </c>
+      <c r="E137" s="103"/>
+    </row>
+    <row r="138" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="101"/>
+      <c r="B138" s="102" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="83" t="s">
-        <v>437</v>
-      </c>
-      <c r="C122" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D122" s="84" t="s">
+      <c r="C138" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D138" s="103" t="s">
         <v>439</v>
       </c>
+      <c r="E138" s="103"/>
+    </row>
+    <row r="139" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="101"/>
+      <c r="B139" s="102" t="s">
+        <v>440</v>
+      </c>
+      <c r="C139" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D139" s="103" t="s">
+        <v>469</v>
+      </c>
+      <c r="E139" s="103"/>
+    </row>
+    <row r="140" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="101"/>
+      <c r="B140" s="102" t="s">
+        <v>441</v>
+      </c>
+      <c r="C140" s="103" t="s">
+        <v>272</v>
+      </c>
+      <c r="D140" s="103" t="s">
+        <v>442</v>
+      </c>
+      <c r="E140" s="103"/>
+    </row>
+    <row r="141" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="101"/>
+      <c r="B141" s="102" t="s">
+        <v>460</v>
+      </c>
+      <c r="C141" s="103" t="s">
+        <v>272</v>
+      </c>
+      <c r="D141" s="103" t="s">
+        <v>461</v>
+      </c>
+      <c r="E141" s="103"/>
+    </row>
+    <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="90"/>
+      <c r="B142" s="91" t="s">
+        <v>471</v>
+      </c>
+      <c r="C142" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D142" s="85" t="s">
+        <v>472</v>
+      </c>
+      <c r="E142" s="85"/>
+    </row>
+    <row r="143" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="90"/>
+      <c r="B143" s="91" t="s">
+        <v>478</v>
+      </c>
+      <c r="C143" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D143" s="85" t="s">
+        <v>479</v>
+      </c>
+      <c r="E143" s="85"/>
+    </row>
+    <row r="144" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="90"/>
+      <c r="B144" s="91" t="s">
+        <v>481</v>
+      </c>
+      <c r="C144" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D144" s="85" t="s">
+        <v>482</v>
+      </c>
+      <c r="E144" s="85"/>
+    </row>
+    <row r="145" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="90"/>
+      <c r="B145" s="91" t="s">
+        <v>483</v>
+      </c>
+      <c r="C145" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D145" s="85" t="s">
+        <v>484</v>
+      </c>
+      <c r="E145" s="85"/>
+    </row>
+    <row r="146" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="96"/>
+      <c r="B146" s="98" t="s">
+        <v>485</v>
+      </c>
+      <c r="C146" s="99" t="s">
+        <v>339</v>
+      </c>
+      <c r="D146" s="99" t="s">
+        <v>486</v>
+      </c>
+      <c r="E146" s="99"/>
+    </row>
+    <row r="147" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="90"/>
+      <c r="B147" s="91" t="s">
+        <v>487</v>
+      </c>
+      <c r="C147" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D147" s="85" t="s">
+        <v>488</v>
+      </c>
+      <c r="E147" s="85"/>
+    </row>
+    <row r="148" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="101"/>
+      <c r="B148" s="102" t="s">
+        <v>490</v>
+      </c>
+      <c r="C148" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D148" s="103" t="s">
+        <v>491</v>
+      </c>
+      <c r="E148" s="103"/>
+    </row>
+    <row r="149" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="101"/>
+      <c r="B149" s="102" t="s">
+        <v>492</v>
+      </c>
+      <c r="C149" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D149" s="103" t="s">
+        <v>493</v>
+      </c>
+      <c r="E149" s="103"/>
+    </row>
+    <row r="150" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="101"/>
+      <c r="B150" s="102" t="s">
+        <v>495</v>
+      </c>
+      <c r="C150" s="103" t="s">
+        <v>339</v>
+      </c>
+      <c r="D150" s="103" t="s">
+        <v>494</v>
+      </c>
+      <c r="E150" s="103"/>
+    </row>
+    <row r="151" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="90"/>
+      <c r="B151" s="91" t="s">
+        <v>496</v>
+      </c>
+      <c r="C151" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D151" s="85" t="s">
+        <v>497</v>
+      </c>
+      <c r="E151" s="85"/>
+    </row>
+    <row r="152" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="90"/>
+      <c r="B152" s="91"/>
+      <c r="C152" s="85"/>
+      <c r="D152" s="85"/>
+      <c r="E152" s="85"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated packaging resources & fixed javafx versions
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Packaging_Resources/lib/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Packaging_Resources/lib/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B334F5F8-B56A-4552-9AC3-EC427696E8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C9CF86-02C9-46AD-817F-6F58F99B60EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="550">
   <si>
     <t>ID</t>
   </si>
@@ -833,9 +833,6 @@
     <t>About ERB</t>
   </si>
   <si>
-    <t>What are indicators of Equitable Resilience?</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
@@ -851,12 +848,6 @@
     <t>19</t>
   </si>
   <si>
-    <t>Goal Setting Scenario</t>
-  </si>
-  <si>
-    <t>Activity To Goal Matching Example</t>
-  </si>
-  <si>
     <t>OutputForm</t>
   </si>
   <si>
@@ -866,9 +857,6 @@
     <t>26</t>
   </si>
   <si>
-    <t>Lay your cards on the table</t>
-  </si>
-  <si>
     <t>27</t>
   </si>
   <si>
@@ -1629,6 +1617,78 @@
   </si>
   <si>
     <t>169 Small</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>Quick Start Guide</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>Additional Resources</t>
+  </si>
+  <si>
+    <t>173</t>
+  </si>
+  <si>
+    <t>The 5 sections of ERB</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>The 5 sections of ERB image</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>How ERB centers equity</t>
+  </si>
+  <si>
+    <t>Supporting materials</t>
+  </si>
+  <si>
+    <t>Indicator card sorting</t>
+  </si>
+  <si>
+    <t>Reflection diary</t>
+  </si>
+  <si>
+    <t>Key takeaways</t>
+  </si>
+  <si>
+    <t>MyPortfolio</t>
+  </si>
+  <si>
+    <t>FAQ</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>Youth Engagement Image: Facilitation Tips</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>Youth Engagement Image: Capacity Considerations</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>Youth Engagement Image: Additional Resources 2</t>
+  </si>
+  <si>
+    <t>Youth Engagement Image: Additional Resources 1</t>
   </si>
 </sst>
 </file>
@@ -1652,7 +1712,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1710,6 +1770,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1967,7 +2045,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2138,42 +2216,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2566,10 +2639,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="107" t="s">
+      <c r="G2" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="108"/>
+      <c r="H2" s="106"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5933,10 +6006,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5960,154 +6033,154 @@
         <v>256</v>
       </c>
       <c r="E1" s="88" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="97"/>
-      <c r="B2" s="93" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="104"/>
+      <c r="B2" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="98" t="s">
+      <c r="C2" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="98"/>
-    </row>
-    <row r="3" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="92"/>
-      <c r="B3" s="93" t="s">
+      <c r="E2" s="97"/>
+    </row>
+    <row r="3" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="96"/>
+      <c r="B3" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D3" s="94" t="s">
-        <v>469</v>
-      </c>
-      <c r="E3" s="94"/>
-    </row>
-    <row r="4" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92"/>
-      <c r="B4" s="93" t="s">
+      <c r="C3" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="85" t="s">
+        <v>465</v>
+      </c>
+      <c r="E3" s="85"/>
+    </row>
+    <row r="4" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="96"/>
+      <c r="B4" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D4" s="94" t="s">
-        <v>474</v>
-      </c>
-      <c r="E4" s="94"/>
-    </row>
-    <row r="5" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="92"/>
-      <c r="B5" s="93" t="s">
+      <c r="C4" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="85" t="s">
+        <v>470</v>
+      </c>
+      <c r="E4" s="85"/>
+    </row>
+    <row r="5" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="96"/>
+      <c r="B5" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D5" s="94" t="s">
+      <c r="C5" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="85" t="s">
+        <v>468</v>
+      </c>
+      <c r="E5" s="85"/>
+    </row>
+    <row r="6" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="96"/>
+      <c r="B6" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="85" t="s">
         <v>472</v>
       </c>
-      <c r="E5" s="94"/>
-    </row>
-    <row r="6" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="92"/>
-      <c r="B6" s="93" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D6" s="94" t="s">
-        <v>476</v>
-      </c>
-      <c r="E6" s="94"/>
-    </row>
-    <row r="7" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="92"/>
-      <c r="B7" s="93" t="s">
+      <c r="E6" s="85"/>
+    </row>
+    <row r="7" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="96"/>
+      <c r="B7" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D7" s="94" t="s">
-        <v>479</v>
-      </c>
-      <c r="E7" s="94"/>
-    </row>
-    <row r="8" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="99"/>
-      <c r="B8" s="100" t="s">
+      <c r="C7" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="85" t="s">
+        <v>475</v>
+      </c>
+      <c r="E7" s="85"/>
+    </row>
+    <row r="8" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="96"/>
+      <c r="B8" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="101" t="s">
-        <v>258</v>
-      </c>
-      <c r="D8" s="101" t="s">
+      <c r="C8" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="85" t="s">
         <v>259</v>
       </c>
-      <c r="E8" s="101"/>
-    </row>
-    <row r="9" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99"/>
-      <c r="B9" s="100" t="s">
+      <c r="E8" s="85"/>
+    </row>
+    <row r="9" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="96"/>
+      <c r="B9" s="91" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="101" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" s="101" t="s">
+      <c r="C9" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="85" t="s">
         <v>261</v>
       </c>
-      <c r="E9" s="101"/>
-    </row>
-    <row r="10" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="99"/>
-      <c r="B10" s="100" t="s">
+      <c r="E9" s="85"/>
+    </row>
+    <row r="10" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="96"/>
+      <c r="B10" s="91" t="s">
         <v>262</v>
       </c>
-      <c r="C10" s="101" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="101" t="s">
+      <c r="C10" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="E10" s="101"/>
-    </row>
-    <row r="11" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="92"/>
-      <c r="B11" s="93" t="s">
+      <c r="E10" s="85"/>
+    </row>
+    <row r="11" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="96"/>
+      <c r="B11" s="91" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D11" s="94" t="s">
-        <v>488</v>
-      </c>
-      <c r="E11" s="94"/>
-    </row>
-    <row r="12" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="99"/>
-      <c r="B12" s="100" t="s">
-        <v>521</v>
-      </c>
-      <c r="C12" s="101" t="s">
-        <v>258</v>
-      </c>
-      <c r="D12" s="101" t="s">
-        <v>522</v>
-      </c>
-      <c r="E12" s="101"/>
+      <c r="C11" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="85" t="s">
+        <v>484</v>
+      </c>
+      <c r="E11" s="85"/>
+    </row>
+    <row r="12" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="96"/>
+      <c r="B12" s="91" t="s">
+        <v>517</v>
+      </c>
+      <c r="C12" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" s="85" t="s">
+        <v>518</v>
+      </c>
+      <c r="E12" s="85"/>
     </row>
     <row r="13" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="90"/>
+      <c r="A13" s="96"/>
       <c r="B13" s="91" t="s">
         <v>157</v>
       </c>
@@ -6115,12 +6188,12 @@
         <v>258</v>
       </c>
       <c r="D13" s="85" t="s">
-        <v>16</v>
+        <v>536</v>
       </c>
       <c r="E13" s="85"/>
     </row>
     <row r="14" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="90"/>
+      <c r="A14" s="96"/>
       <c r="B14" s="91" t="s">
         <v>158</v>
       </c>
@@ -6128,12 +6201,12 @@
         <v>258</v>
       </c>
       <c r="D14" s="85" t="s">
-        <v>17</v>
+        <v>196</v>
       </c>
       <c r="E14" s="85"/>
     </row>
     <row r="15" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="90"/>
+      <c r="A15" s="96"/>
       <c r="B15" s="91" t="s">
         <v>159</v>
       </c>
@@ -6141,12 +6214,12 @@
         <v>258</v>
       </c>
       <c r="D15" s="85" t="s">
-        <v>264</v>
+        <v>537</v>
       </c>
       <c r="E15" s="85"/>
     </row>
     <row r="16" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="90"/>
+      <c r="A16" s="96"/>
       <c r="B16" s="91" t="s">
         <v>160</v>
       </c>
@@ -6159,72 +6232,72 @@
       <c r="E16" s="85"/>
     </row>
     <row r="17" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="90"/>
+      <c r="A17" s="96"/>
       <c r="B17" s="91" t="s">
+        <v>264</v>
+      </c>
+      <c r="C17" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="85" t="s">
+        <v>439</v>
+      </c>
+      <c r="E17" s="85"/>
+    </row>
+    <row r="18" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="96"/>
+      <c r="B18" s="91" t="s">
         <v>265</v>
       </c>
-      <c r="C17" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D17" s="85" t="s">
-        <v>443</v>
-      </c>
-      <c r="E17" s="85"/>
-    </row>
-    <row r="18" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="90"/>
-      <c r="B18" s="91" t="s">
+      <c r="C18" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="85" t="s">
+        <v>444</v>
+      </c>
+      <c r="E18" s="85"/>
+    </row>
+    <row r="19" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="96"/>
+      <c r="B19" s="91" t="s">
         <v>266</v>
       </c>
-      <c r="C18" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="85" t="s">
-        <v>448</v>
-      </c>
-      <c r="E18" s="85"/>
-    </row>
-    <row r="19" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="90"/>
-      <c r="B19" s="91" t="s">
+      <c r="C19" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="85" t="s">
+        <v>449</v>
+      </c>
+      <c r="E19" s="85"/>
+    </row>
+    <row r="20" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="96"/>
+      <c r="B20" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="C19" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D19" s="85" t="s">
-        <v>453</v>
-      </c>
-      <c r="E19" s="85"/>
-    </row>
-    <row r="20" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="90"/>
-      <c r="B20" s="91" t="s">
+      <c r="C20" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="85" t="s">
+        <v>458</v>
+      </c>
+      <c r="E20" s="85"/>
+    </row>
+    <row r="21" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="96"/>
+      <c r="B21" s="91" t="s">
         <v>268</v>
       </c>
-      <c r="C20" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="85" t="s">
+      <c r="C21" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="85" t="s">
         <v>462</v>
       </c>
-      <c r="E20" s="85"/>
-    </row>
-    <row r="21" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="90"/>
-      <c r="B21" s="91" t="s">
-        <v>269</v>
-      </c>
-      <c r="C21" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D21" s="85" t="s">
-        <v>466</v>
-      </c>
       <c r="E21" s="85"/>
     </row>
     <row r="22" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="90"/>
+      <c r="A22" s="96"/>
       <c r="B22" s="91" t="s">
         <v>153</v>
       </c>
@@ -6232,12 +6305,12 @@
         <v>258</v>
       </c>
       <c r="D22" s="85" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="E22" s="85"/>
     </row>
     <row r="23" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="90"/>
+      <c r="A23" s="96"/>
       <c r="B23" s="91" t="s">
         <v>161</v>
       </c>
@@ -6245,12 +6318,12 @@
         <v>258</v>
       </c>
       <c r="D23" s="85" t="s">
-        <v>270</v>
+        <v>538</v>
       </c>
       <c r="E23" s="85"/>
     </row>
     <row r="24" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="90"/>
+      <c r="A24" s="96"/>
       <c r="B24" s="91" t="s">
         <v>162</v>
       </c>
@@ -6258,12 +6331,12 @@
         <v>258</v>
       </c>
       <c r="D24" s="85" t="s">
-        <v>271</v>
+        <v>539</v>
       </c>
       <c r="E24" s="85"/>
     </row>
     <row r="25" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="90"/>
+      <c r="A25" s="96"/>
       <c r="B25" s="91" t="s">
         <v>163</v>
       </c>
@@ -6271,25 +6344,25 @@
         <v>258</v>
       </c>
       <c r="D25" s="85" t="s">
-        <v>8</v>
+        <v>540</v>
       </c>
       <c r="E25" s="85"/>
     </row>
     <row r="26" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="90"/>
+      <c r="A26" s="96"/>
       <c r="B26" s="91" t="s">
         <v>164</v>
       </c>
       <c r="C26" s="85" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D26" s="85" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E26" s="85"/>
     </row>
     <row r="27" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="90"/>
+      <c r="A27" s="96"/>
       <c r="B27" s="91" t="s">
         <v>165</v>
       </c>
@@ -6297,64 +6370,64 @@
         <v>258</v>
       </c>
       <c r="D27" s="85" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="E27" s="85"/>
     </row>
     <row r="28" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="90"/>
+      <c r="A28" s="96"/>
       <c r="B28" s="91" t="s">
+        <v>271</v>
+      </c>
+      <c r="C28" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D28" s="85" t="s">
+        <v>541</v>
+      </c>
+      <c r="E28" s="85"/>
+    </row>
+    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="96"/>
+      <c r="B29" s="91" t="s">
+        <v>272</v>
+      </c>
+      <c r="C29" s="85" t="s">
+        <v>275</v>
+      </c>
+      <c r="D29" s="85" t="s">
+        <v>273</v>
+      </c>
+      <c r="E29" s="85"/>
+    </row>
+    <row r="30" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="96"/>
+      <c r="B30" s="91" t="s">
         <v>274</v>
       </c>
-      <c r="C28" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D28" s="85" t="s">
+      <c r="C30" s="85" t="s">
         <v>275</v>
       </c>
-      <c r="E28" s="85"/>
-    </row>
-    <row r="29" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="109"/>
-      <c r="B29" s="110" t="s">
+      <c r="D30" s="85" t="s">
+        <v>233</v>
+      </c>
+      <c r="E30" s="85"/>
+    </row>
+    <row r="31" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="96"/>
+      <c r="B31" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="C29" s="111" t="s">
-        <v>279</v>
-      </c>
-      <c r="D29" s="111" t="s">
-        <v>277</v>
-      </c>
-      <c r="E29" s="111"/>
-    </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="109"/>
-      <c r="B30" s="110" t="s">
-        <v>278</v>
-      </c>
-      <c r="C30" s="111" t="s">
-        <v>279</v>
-      </c>
-      <c r="D30" s="111" t="s">
-        <v>233</v>
-      </c>
-      <c r="E30" s="111"/>
-    </row>
-    <row r="31" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="109"/>
-      <c r="B31" s="110" t="s">
-        <v>280</v>
-      </c>
-      <c r="C31" s="111" t="s">
-        <v>279</v>
-      </c>
-      <c r="D31" s="111" t="s">
+      <c r="C31" s="85" t="s">
+        <v>275</v>
+      </c>
+      <c r="D31" s="85" t="s">
         <v>234</v>
       </c>
-      <c r="E31" s="111"/>
+      <c r="E31" s="85"/>
     </row>
     <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="90"/>
+      <c r="A32" s="96"/>
       <c r="B32" s="91" t="s">
         <v>154</v>
       </c>
@@ -6362,12 +6435,12 @@
         <v>258</v>
       </c>
       <c r="D32" s="85" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="E32" s="85"/>
     </row>
     <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="90"/>
+      <c r="A33" s="96"/>
       <c r="B33" s="91" t="s">
         <v>166</v>
       </c>
@@ -6375,12 +6448,12 @@
         <v>258</v>
       </c>
       <c r="D33" s="85" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="E33" s="85"/>
     </row>
     <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="90"/>
+      <c r="A34" s="96"/>
       <c r="B34" s="91" t="s">
         <v>167</v>
       </c>
@@ -6393,7 +6466,7 @@
       <c r="E34" s="85"/>
     </row>
     <row r="35" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="90"/>
+      <c r="A35" s="96"/>
       <c r="B35" s="91" t="s">
         <v>168</v>
       </c>
@@ -6401,12 +6474,12 @@
         <v>258</v>
       </c>
       <c r="D35" s="85" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="E35" s="85"/>
     </row>
     <row r="36" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="90"/>
+      <c r="A36" s="96"/>
       <c r="B36" s="91" t="s">
         <v>169</v>
       </c>
@@ -6414,12 +6487,12 @@
         <v>258</v>
       </c>
       <c r="D36" s="85" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E36" s="85"/>
     </row>
     <row r="37" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="90"/>
+      <c r="A37" s="96"/>
       <c r="B37" s="91" t="s">
         <v>170</v>
       </c>
@@ -6427,12 +6500,12 @@
         <v>258</v>
       </c>
       <c r="D37" s="85" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E37" s="85"/>
     </row>
     <row r="38" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="90"/>
+      <c r="A38" s="96"/>
       <c r="B38" s="91" t="s">
         <v>171</v>
       </c>
@@ -6440,12 +6513,12 @@
         <v>258</v>
       </c>
       <c r="D38" s="85" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E38" s="85"/>
     </row>
     <row r="39" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="90"/>
+      <c r="A39" s="96"/>
       <c r="B39" s="91" t="s">
         <v>172</v>
       </c>
@@ -6453,285 +6526,285 @@
         <v>258</v>
       </c>
       <c r="D39" s="85" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E39" s="85"/>
     </row>
     <row r="40" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="90"/>
+      <c r="A40" s="96"/>
       <c r="B40" s="91" t="s">
+        <v>278</v>
+      </c>
+      <c r="C40" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D40" s="85" t="s">
+        <v>447</v>
+      </c>
+      <c r="E40" s="85"/>
+    </row>
+    <row r="41" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="98"/>
+      <c r="B41" s="99" t="s">
+        <v>279</v>
+      </c>
+      <c r="C41" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D41" s="100" t="s">
+        <v>280</v>
+      </c>
+      <c r="E41" s="100"/>
+    </row>
+    <row r="42" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="98"/>
+      <c r="B42" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D42" s="100" t="s">
+        <v>281</v>
+      </c>
+      <c r="E42" s="100"/>
+    </row>
+    <row r="43" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="98"/>
+      <c r="B43" s="99" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D43" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="100"/>
+    </row>
+    <row r="44" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="98"/>
+      <c r="B44" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="C44" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D44" s="100" t="s">
         <v>282</v>
       </c>
-      <c r="C40" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D40" s="85" t="s">
-        <v>451</v>
-      </c>
-      <c r="E40" s="85"/>
-    </row>
-    <row r="41" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="90"/>
-      <c r="B41" s="91" t="s">
+      <c r="E44" s="100"/>
+    </row>
+    <row r="45" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="98"/>
+      <c r="B45" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="100" t="s">
         <v>283</v>
       </c>
-      <c r="C41" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D41" s="85" t="s">
+      <c r="E45" s="100"/>
+    </row>
+    <row r="46" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="98"/>
+      <c r="B46" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="C46" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D46" s="100" t="s">
         <v>284</v>
       </c>
-      <c r="E41" s="85"/>
-    </row>
-    <row r="42" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="90"/>
-      <c r="B42" s="91" t="s">
-        <v>155</v>
-      </c>
-      <c r="C42" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D42" s="85" t="s">
+      <c r="E46" s="100"/>
+    </row>
+    <row r="47" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="98"/>
+      <c r="B47" s="99" t="s">
         <v>285</v>
       </c>
-      <c r="E42" s="85"/>
-    </row>
-    <row r="43" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="90"/>
-      <c r="B43" s="91" t="s">
-        <v>174</v>
-      </c>
-      <c r="C43" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D43" s="85" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="85"/>
-    </row>
-    <row r="44" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="90"/>
-      <c r="B44" s="91" t="s">
-        <v>175</v>
-      </c>
-      <c r="C44" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D44" s="85" t="s">
+      <c r="C47" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="100" t="s">
         <v>286</v>
       </c>
-      <c r="E44" s="85"/>
-    </row>
-    <row r="45" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="90"/>
-      <c r="B45" s="91" t="s">
-        <v>176</v>
-      </c>
-      <c r="C45" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D45" s="85" t="s">
+      <c r="E47" s="100"/>
+    </row>
+    <row r="48" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="98"/>
+      <c r="B48" s="99" t="s">
         <v>287</v>
       </c>
-      <c r="E45" s="85"/>
-    </row>
-    <row r="46" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="90"/>
-      <c r="B46" s="91" t="s">
-        <v>177</v>
-      </c>
-      <c r="C46" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D46" s="85" t="s">
+      <c r="C48" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" s="100" t="s">
         <v>288</v>
       </c>
-      <c r="E46" s="85"/>
-    </row>
-    <row r="47" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="90"/>
-      <c r="B47" s="91" t="s">
+      <c r="E48" s="100"/>
+    </row>
+    <row r="49" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="98"/>
+      <c r="B49" s="99" t="s">
         <v>289</v>
       </c>
-      <c r="C47" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D47" s="85" t="s">
+      <c r="C49" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D49" s="100" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="100"/>
+    </row>
+    <row r="50" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="98"/>
+      <c r="B50" s="99" t="s">
         <v>290</v>
       </c>
-      <c r="E47" s="85"/>
-    </row>
-    <row r="48" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="90"/>
-      <c r="B48" s="91" t="s">
+      <c r="C50" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="100"/>
+    </row>
+    <row r="51" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="98"/>
+      <c r="B51" s="99" t="s">
         <v>291</v>
       </c>
-      <c r="C48" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D48" s="85" t="s">
+      <c r="C51" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" s="100" t="s">
         <v>292</v>
       </c>
-      <c r="E48" s="85"/>
-    </row>
-    <row r="49" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="90"/>
-      <c r="B49" s="91" t="s">
+      <c r="E51" s="100"/>
+    </row>
+    <row r="52" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="98"/>
+      <c r="B52" s="99" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D52" s="100" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="100"/>
+    </row>
+    <row r="53" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="98"/>
+      <c r="B53" s="99" t="s">
+        <v>178</v>
+      </c>
+      <c r="C53" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D53" s="100" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" s="100"/>
+    </row>
+    <row r="54" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="98"/>
+      <c r="B54" s="99" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D54" s="100" t="s">
         <v>293</v>
       </c>
-      <c r="C49" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D49" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" s="85"/>
-    </row>
-    <row r="50" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="90"/>
-      <c r="B50" s="91" t="s">
+      <c r="E54" s="100"/>
+    </row>
+    <row r="55" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="98"/>
+      <c r="B55" s="99" t="s">
+        <v>180</v>
+      </c>
+      <c r="C55" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D55" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="100"/>
+    </row>
+    <row r="56" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="98"/>
+      <c r="B56" s="99" t="s">
+        <v>181</v>
+      </c>
+      <c r="C56" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D56" s="100" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" s="100"/>
+    </row>
+    <row r="57" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="98"/>
+      <c r="B57" s="99" t="s">
+        <v>182</v>
+      </c>
+      <c r="C57" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D57" s="100" t="s">
         <v>294</v>
       </c>
-      <c r="C50" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D50" s="85" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" s="85"/>
-    </row>
-    <row r="51" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="90"/>
-      <c r="B51" s="91" t="s">
+      <c r="E57" s="100"/>
+    </row>
+    <row r="58" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="98"/>
+      <c r="B58" s="99" t="s">
+        <v>183</v>
+      </c>
+      <c r="C58" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D58" s="100" t="s">
         <v>295</v>
       </c>
-      <c r="C51" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D51" s="85" t="s">
+      <c r="E58" s="100"/>
+    </row>
+    <row r="59" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="98"/>
+      <c r="B59" s="99" t="s">
+        <v>184</v>
+      </c>
+      <c r="C59" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D59" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="100"/>
+    </row>
+    <row r="60" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="98"/>
+      <c r="B60" s="99" t="s">
+        <v>185</v>
+      </c>
+      <c r="C60" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="100" t="s">
         <v>296</v>
       </c>
-      <c r="E51" s="85"/>
-    </row>
-    <row r="52" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="90"/>
-      <c r="B52" s="91" t="s">
-        <v>156</v>
-      </c>
-      <c r="C52" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" s="85" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" s="85"/>
-    </row>
-    <row r="53" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="90"/>
-      <c r="B53" s="91" t="s">
-        <v>178</v>
-      </c>
-      <c r="C53" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D53" s="85" t="s">
-        <v>28</v>
-      </c>
-      <c r="E53" s="85"/>
-    </row>
-    <row r="54" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="90"/>
-      <c r="B54" s="91" t="s">
-        <v>179</v>
-      </c>
-      <c r="C54" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D54" s="85" t="s">
-        <v>297</v>
-      </c>
-      <c r="E54" s="85"/>
-    </row>
-    <row r="55" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="90"/>
-      <c r="B55" s="91" t="s">
-        <v>180</v>
-      </c>
-      <c r="C55" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D55" s="85" t="s">
-        <v>30</v>
-      </c>
-      <c r="E55" s="85"/>
-    </row>
-    <row r="56" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="90"/>
-      <c r="B56" s="91" t="s">
-        <v>181</v>
-      </c>
-      <c r="C56" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D56" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="E56" s="85"/>
-    </row>
-    <row r="57" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="90"/>
-      <c r="B57" s="91" t="s">
-        <v>182</v>
-      </c>
-      <c r="C57" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D57" s="85" t="s">
-        <v>298</v>
-      </c>
-      <c r="E57" s="85"/>
-    </row>
-    <row r="58" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="90"/>
-      <c r="B58" s="91" t="s">
-        <v>183</v>
-      </c>
-      <c r="C58" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D58" s="85" t="s">
-        <v>299</v>
-      </c>
-      <c r="E58" s="85"/>
-    </row>
-    <row r="59" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="90"/>
-      <c r="B59" s="91" t="s">
-        <v>184</v>
-      </c>
-      <c r="C59" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D59" s="85" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="85"/>
-    </row>
-    <row r="60" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="90"/>
-      <c r="B60" s="91" t="s">
-        <v>185</v>
-      </c>
-      <c r="C60" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D60" s="85" t="s">
-        <v>300</v>
-      </c>
-      <c r="E60" s="85"/>
+      <c r="E60" s="100"/>
     </row>
     <row r="61" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="90"/>
+      <c r="A61" s="96"/>
       <c r="B61" s="91" t="s">
         <v>186</v>
       </c>
@@ -6739,27 +6812,27 @@
         <v>258</v>
       </c>
       <c r="D61" s="85" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="E61" s="85"/>
     </row>
     <row r="62" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="90"/>
+      <c r="A62" s="96"/>
       <c r="B62" s="91" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C62" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D62" s="85" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E62" s="85"/>
     </row>
     <row r="63" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="90"/>
+      <c r="A63" s="96"/>
       <c r="B63" s="91" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C63" s="85" t="s">
         <v>258</v>
@@ -6770,155 +6843,155 @@
       <c r="E63" s="85"/>
     </row>
     <row r="64" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="90"/>
+      <c r="A64" s="95"/>
       <c r="B64" s="91" t="s">
+        <v>300</v>
+      </c>
+      <c r="C64" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D64" s="85" t="s">
+        <v>302</v>
+      </c>
+      <c r="E64" s="85"/>
+    </row>
+    <row r="65" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="95"/>
+      <c r="B65" s="91" t="s">
+        <v>303</v>
+      </c>
+      <c r="C65" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D65" s="85" t="s">
         <v>304</v>
       </c>
-      <c r="C64" s="85" t="s">
+      <c r="E65" s="85"/>
+    </row>
+    <row r="66" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="95"/>
+      <c r="B66" s="91" t="s">
         <v>305</v>
       </c>
-      <c r="D64" s="85" t="s">
+      <c r="C66" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D66" s="85" t="s">
         <v>306</v>
       </c>
-      <c r="E64" s="85"/>
-    </row>
-    <row r="65" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="90"/>
-      <c r="B65" s="91" t="s">
+      <c r="E66" s="85"/>
+    </row>
+    <row r="67" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="95"/>
+      <c r="B67" s="91" t="s">
         <v>307</v>
       </c>
-      <c r="C65" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D65" s="85" t="s">
+      <c r="C67" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D67" s="85" t="s">
         <v>308</v>
       </c>
-      <c r="E65" s="85"/>
-    </row>
-    <row r="66" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="90"/>
-      <c r="B66" s="91" t="s">
+      <c r="E67" s="85"/>
+    </row>
+    <row r="68" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="95"/>
+      <c r="B68" s="91" t="s">
         <v>309</v>
       </c>
-      <c r="C66" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D66" s="85" t="s">
+      <c r="C68" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D68" s="85" t="s">
         <v>310</v>
       </c>
-      <c r="E66" s="85"/>
-    </row>
-    <row r="67" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="90"/>
-      <c r="B67" s="91" t="s">
+      <c r="E68" s="85"/>
+    </row>
+    <row r="69" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="95"/>
+      <c r="B69" s="91" t="s">
         <v>311</v>
       </c>
-      <c r="C67" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D67" s="85" t="s">
+      <c r="C69" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D69" s="85" t="s">
         <v>312</v>
       </c>
-      <c r="E67" s="85"/>
-    </row>
-    <row r="68" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="90"/>
-      <c r="B68" s="91" t="s">
+      <c r="E69" s="85"/>
+    </row>
+    <row r="70" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="95"/>
+      <c r="B70" s="91" t="s">
         <v>313</v>
       </c>
-      <c r="C68" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D68" s="85" t="s">
+      <c r="C70" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D70" s="85" t="s">
         <v>314</v>
       </c>
-      <c r="E68" s="85"/>
-    </row>
-    <row r="69" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="90"/>
-      <c r="B69" s="91" t="s">
+      <c r="E70" s="85"/>
+    </row>
+    <row r="71" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="95"/>
+      <c r="B71" s="91" t="s">
         <v>315</v>
       </c>
-      <c r="C69" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D69" s="85" t="s">
+      <c r="C71" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D71" s="85" t="s">
         <v>316</v>
       </c>
-      <c r="E69" s="85"/>
-    </row>
-    <row r="70" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="90"/>
-      <c r="B70" s="91" t="s">
+      <c r="E71" s="85"/>
+    </row>
+    <row r="72" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="95"/>
+      <c r="B72" s="91" t="s">
         <v>317</v>
       </c>
-      <c r="C70" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D70" s="85" t="s">
+      <c r="C72" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D72" s="85" t="s">
         <v>318</v>
       </c>
-      <c r="E70" s="85"/>
-    </row>
-    <row r="71" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="90"/>
-      <c r="B71" s="91" t="s">
+      <c r="E72" s="85"/>
+    </row>
+    <row r="73" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="98"/>
+      <c r="B73" s="99" t="s">
         <v>319</v>
       </c>
-      <c r="C71" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D71" s="85" t="s">
+      <c r="C73" s="100" t="s">
+        <v>301</v>
+      </c>
+      <c r="D73" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="E71" s="85"/>
-    </row>
-    <row r="72" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="90"/>
-      <c r="B72" s="91" t="s">
+      <c r="E73" s="100"/>
+    </row>
+    <row r="74" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="95"/>
+      <c r="B74" s="91" t="s">
         <v>321</v>
       </c>
-      <c r="C72" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D72" s="85" t="s">
+      <c r="C74" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D74" s="85" t="s">
         <v>322</v>
       </c>
-      <c r="E72" s="85"/>
-    </row>
-    <row r="73" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="90"/>
-      <c r="B73" s="91" t="s">
+      <c r="E74" s="85"/>
+    </row>
+    <row r="75" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="95"/>
+      <c r="B75" s="91" t="s">
         <v>323</v>
       </c>
-      <c r="C73" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D73" s="85" t="s">
-        <v>324</v>
-      </c>
-      <c r="E73" s="85"/>
-    </row>
-    <row r="74" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="90"/>
-      <c r="B74" s="91" t="s">
-        <v>325</v>
-      </c>
-      <c r="C74" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D74" s="85" t="s">
-        <v>326</v>
-      </c>
-      <c r="E74" s="85"/>
-    </row>
-    <row r="75" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="90"/>
-      <c r="B75" s="91" t="s">
-        <v>327</v>
-      </c>
       <c r="C75" s="85" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D75" s="85" t="s">
         <v>221</v>
@@ -6926,116 +6999,116 @@
       <c r="E75" s="85"/>
     </row>
     <row r="76" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="90"/>
+      <c r="A76" s="95"/>
       <c r="B76" s="91" t="s">
+        <v>324</v>
+      </c>
+      <c r="C76" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D76" s="85" t="s">
+        <v>325</v>
+      </c>
+      <c r="E76" s="85"/>
+    </row>
+    <row r="77" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="95"/>
+      <c r="B77" s="91" t="s">
+        <v>326</v>
+      </c>
+      <c r="C77" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D77" s="85" t="s">
+        <v>327</v>
+      </c>
+      <c r="E77" s="85"/>
+    </row>
+    <row r="78" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="95"/>
+      <c r="B78" s="91" t="s">
         <v>328</v>
       </c>
-      <c r="C76" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D76" s="85" t="s">
+      <c r="C78" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D78" s="85" t="s">
         <v>329</v>
       </c>
-      <c r="E76" s="85"/>
-    </row>
-    <row r="77" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="90"/>
-      <c r="B77" s="91" t="s">
+      <c r="E78" s="85"/>
+    </row>
+    <row r="79" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="95"/>
+      <c r="B79" s="91" t="s">
         <v>330</v>
       </c>
-      <c r="C77" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D77" s="85" t="s">
+      <c r="C79" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D79" s="85" t="s">
         <v>331</v>
       </c>
-      <c r="E77" s="85"/>
-    </row>
-    <row r="78" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="90"/>
-      <c r="B78" s="91" t="s">
+      <c r="E79" s="85"/>
+    </row>
+    <row r="80" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="95"/>
+      <c r="B80" s="91" t="s">
         <v>332</v>
       </c>
-      <c r="C78" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D78" s="85" t="s">
+      <c r="C80" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D80" s="85" t="s">
         <v>333</v>
       </c>
-      <c r="E78" s="85"/>
-    </row>
-    <row r="79" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="90"/>
-      <c r="B79" s="91" t="s">
+      <c r="E80" s="85"/>
+    </row>
+    <row r="81" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="95"/>
+      <c r="B81" s="91" t="s">
         <v>334</v>
       </c>
-      <c r="C79" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D79" s="85" t="s">
+      <c r="C81" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="E79" s="85"/>
-    </row>
-    <row r="80" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="90"/>
-      <c r="B80" s="91" t="s">
+      <c r="D81" s="85" t="s">
         <v>336</v>
       </c>
-      <c r="C80" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D80" s="85" t="s">
+      <c r="E81" s="85"/>
+    </row>
+    <row r="82" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="95"/>
+      <c r="B82" s="91" t="s">
         <v>337</v>
       </c>
-      <c r="E80" s="85"/>
-    </row>
-    <row r="81" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="90"/>
-      <c r="B81" s="91" t="s">
+      <c r="C82" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D82" s="85" t="s">
         <v>338</v>
       </c>
-      <c r="C81" s="85" t="s">
+      <c r="E82" s="85"/>
+    </row>
+    <row r="83" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="95"/>
+      <c r="B83" s="91" t="s">
         <v>339</v>
       </c>
-      <c r="D81" s="85" t="s">
+      <c r="C83" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D83" s="85" t="s">
         <v>340</v>
       </c>
-      <c r="E81" s="85"/>
-    </row>
-    <row r="82" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="90"/>
-      <c r="B82" s="91" t="s">
+      <c r="E83" s="85"/>
+    </row>
+    <row r="84" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="95"/>
+      <c r="B84" s="91" t="s">
         <v>341</v>
       </c>
-      <c r="C82" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D82" s="85" t="s">
-        <v>342</v>
-      </c>
-      <c r="E82" s="85"/>
-    </row>
-    <row r="83" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="90"/>
-      <c r="B83" s="91" t="s">
-        <v>343</v>
-      </c>
-      <c r="C83" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D83" s="85" t="s">
-        <v>344</v>
-      </c>
-      <c r="E83" s="85"/>
-    </row>
-    <row r="84" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="90"/>
-      <c r="B84" s="91" t="s">
-        <v>345</v>
-      </c>
       <c r="C84" s="85" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D84" s="85" t="s">
         <v>233</v>
@@ -7043,12 +7116,12 @@
       <c r="E84" s="85"/>
     </row>
     <row r="85" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="90"/>
+      <c r="A85" s="95"/>
       <c r="B85" s="91" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C85" s="85" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D85" s="85" t="s">
         <v>234</v>
@@ -7056,322 +7129,322 @@
       <c r="E85" s="85"/>
     </row>
     <row r="86" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="90"/>
+      <c r="A86" s="95"/>
       <c r="B86" s="91" t="s">
+        <v>343</v>
+      </c>
+      <c r="C86" s="85" t="s">
+        <v>344</v>
+      </c>
+      <c r="D86" s="85" t="s">
+        <v>345</v>
+      </c>
+      <c r="E86" s="85" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="95"/>
+      <c r="B87" s="91" t="s">
+        <v>346</v>
+      </c>
+      <c r="C87" s="85" t="s">
+        <v>344</v>
+      </c>
+      <c r="D87" s="85" t="s">
         <v>347</v>
       </c>
-      <c r="C86" s="85" t="s">
+      <c r="E87" s="85" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="98"/>
+      <c r="B88" s="99" t="s">
+        <v>349</v>
+      </c>
+      <c r="C88" s="100" t="s">
         <v>348</v>
       </c>
-      <c r="D86" s="85" t="s">
-        <v>349</v>
-      </c>
-      <c r="E86" s="85" t="s">
+      <c r="D88" s="100" t="s">
+        <v>193</v>
+      </c>
+      <c r="E88" s="102" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="98"/>
+      <c r="B89" s="99" t="s">
+        <v>350</v>
+      </c>
+      <c r="C89" s="100" t="s">
+        <v>348</v>
+      </c>
+      <c r="D89" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="E89" s="102" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="98"/>
+      <c r="B90" s="99" t="s">
+        <v>351</v>
+      </c>
+      <c r="C90" s="100" t="s">
+        <v>348</v>
+      </c>
+      <c r="D90" s="100" t="s">
+        <v>81</v>
+      </c>
+      <c r="E90" s="102" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="98"/>
+      <c r="B91" s="99" t="s">
+        <v>352</v>
+      </c>
+      <c r="C91" s="100" t="s">
+        <v>348</v>
+      </c>
+      <c r="D91" s="100" t="s">
+        <v>82</v>
+      </c>
+      <c r="E91" s="102" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="98"/>
+      <c r="B92" s="99" t="s">
+        <v>353</v>
+      </c>
+      <c r="C92" s="100" t="s">
+        <v>348</v>
+      </c>
+      <c r="D92" s="100" t="s">
+        <v>354</v>
+      </c>
+      <c r="E92" s="102" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="98"/>
+      <c r="B93" s="99" t="s">
+        <v>356</v>
+      </c>
+      <c r="C93" s="100" t="s">
+        <v>348</v>
+      </c>
+      <c r="D93" s="100" t="s">
+        <v>357</v>
+      </c>
+      <c r="E93" s="102" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="96"/>
+      <c r="B94" s="91" t="s">
+        <v>359</v>
+      </c>
+      <c r="C94" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="E94" s="85"/>
+    </row>
+    <row r="95" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="96"/>
+      <c r="B95" s="91" t="s">
+        <v>361</v>
+      </c>
+      <c r="C95" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="85" t="s">
+        <v>450</v>
+      </c>
+      <c r="E95" s="85"/>
+    </row>
+    <row r="96" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="96"/>
+      <c r="B96" s="91" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="90"/>
-      <c r="B87" s="91" t="s">
-        <v>350</v>
-      </c>
-      <c r="C87" s="85" t="s">
-        <v>348</v>
-      </c>
-      <c r="D87" s="85" t="s">
-        <v>351</v>
-      </c>
-      <c r="E87" s="85" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="90"/>
-      <c r="B88" s="91" t="s">
-        <v>353</v>
-      </c>
-      <c r="C88" s="85" t="s">
-        <v>352</v>
-      </c>
-      <c r="D88" s="85" t="s">
-        <v>193</v>
-      </c>
-      <c r="E88" s="96" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="90"/>
-      <c r="B89" s="91" t="s">
-        <v>354</v>
-      </c>
-      <c r="C89" s="85" t="s">
-        <v>352</v>
-      </c>
-      <c r="D89" s="85" t="s">
-        <v>80</v>
-      </c>
-      <c r="E89" s="96" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="90"/>
-      <c r="B90" s="91" t="s">
-        <v>355</v>
-      </c>
-      <c r="C90" s="85" t="s">
-        <v>352</v>
-      </c>
-      <c r="D90" s="85" t="s">
-        <v>81</v>
-      </c>
-      <c r="E90" s="96" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="90"/>
-      <c r="B91" s="91" t="s">
-        <v>356</v>
-      </c>
-      <c r="C91" s="85" t="s">
-        <v>352</v>
-      </c>
-      <c r="D91" s="85" t="s">
-        <v>82</v>
-      </c>
-      <c r="E91" s="96" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="90"/>
-      <c r="B92" s="91" t="s">
-        <v>357</v>
-      </c>
-      <c r="C92" s="85" t="s">
-        <v>352</v>
-      </c>
-      <c r="D92" s="85" t="s">
-        <v>358</v>
-      </c>
-      <c r="E92" s="96" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="90"/>
-      <c r="B93" s="91" t="s">
-        <v>360</v>
-      </c>
-      <c r="C93" s="85" t="s">
-        <v>352</v>
-      </c>
-      <c r="D93" s="85" t="s">
-        <v>361</v>
-      </c>
-      <c r="E93" s="96" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="90"/>
-      <c r="B94" s="91" t="s">
+      <c r="C96" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D96" s="85" t="s">
         <v>363</v>
       </c>
-      <c r="C94" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D94" s="85" t="s">
+      <c r="E96" s="85"/>
+    </row>
+    <row r="97" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="96"/>
+      <c r="B97" s="91" t="s">
         <v>364</v>
       </c>
-      <c r="E94" s="85"/>
-    </row>
-    <row r="95" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="90"/>
-      <c r="B95" s="91" t="s">
+      <c r="C97" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D97" s="85" t="s">
         <v>365</v>
       </c>
-      <c r="C95" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D95" s="85" t="s">
-        <v>454</v>
-      </c>
-      <c r="E95" s="85"/>
-    </row>
-    <row r="96" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="90"/>
-      <c r="B96" s="91" t="s">
+      <c r="E97" s="85"/>
+    </row>
+    <row r="98" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="96"/>
+      <c r="B98" s="91" t="s">
         <v>366</v>
       </c>
-      <c r="C96" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D96" s="85" t="s">
+      <c r="C98" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" s="85" t="s">
         <v>367</v>
       </c>
-      <c r="E96" s="85"/>
-    </row>
-    <row r="97" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="90"/>
-      <c r="B97" s="91" t="s">
+      <c r="E98" s="85"/>
+    </row>
+    <row r="99" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="96"/>
+      <c r="B99" s="91" t="s">
         <v>368</v>
       </c>
-      <c r="C97" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D97" s="85" t="s">
+      <c r="C99" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D99" s="85" t="s">
         <v>369</v>
       </c>
-      <c r="E97" s="85"/>
-    </row>
-    <row r="98" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="90"/>
-      <c r="B98" s="91" t="s">
+      <c r="E99" s="85"/>
+    </row>
+    <row r="100" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="96"/>
+      <c r="B100" s="91" t="s">
         <v>370</v>
       </c>
-      <c r="C98" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D98" s="85" t="s">
+      <c r="C100" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" s="85" t="s">
         <v>371</v>
       </c>
-      <c r="E98" s="85"/>
-    </row>
-    <row r="99" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="90"/>
-      <c r="B99" s="91" t="s">
-        <v>372</v>
-      </c>
-      <c r="C99" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D99" s="85" t="s">
-        <v>373</v>
-      </c>
-      <c r="E99" s="85"/>
-    </row>
-    <row r="100" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="90"/>
-      <c r="B100" s="91" t="s">
+      <c r="E100" s="85"/>
+    </row>
+    <row r="101" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="96"/>
+      <c r="B101" s="91" t="s">
         <v>374</v>
       </c>
-      <c r="C100" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D100" s="85" t="s">
+      <c r="C101" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" s="85" t="s">
         <v>375</v>
       </c>
-      <c r="E100" s="85"/>
-    </row>
-    <row r="101" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="90"/>
-      <c r="B101" s="91" t="s">
+      <c r="E101" s="85"/>
+    </row>
+    <row r="102" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="96"/>
+      <c r="B102" s="91" t="s">
+        <v>376</v>
+      </c>
+      <c r="C102" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D102" s="85" t="s">
+        <v>377</v>
+      </c>
+      <c r="E102" s="85"/>
+    </row>
+    <row r="103" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="96"/>
+      <c r="B103" s="91" t="s">
         <v>378</v>
       </c>
-      <c r="C101" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D101" s="85" t="s">
+      <c r="C103" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" s="85" t="s">
         <v>379</v>
       </c>
-      <c r="E101" s="85"/>
-    </row>
-    <row r="102" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="90"/>
-      <c r="B102" s="91" t="s">
+      <c r="E103" s="85"/>
+    </row>
+    <row r="104" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="96"/>
+      <c r="B104" s="91" t="s">
         <v>380</v>
       </c>
-      <c r="C102" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D102" s="85" t="s">
+      <c r="C104" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D104" s="85" t="s">
+        <v>451</v>
+      </c>
+      <c r="E104" s="85"/>
+    </row>
+    <row r="105" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="96"/>
+      <c r="B105" s="91" t="s">
         <v>381</v>
       </c>
-      <c r="E102" s="85"/>
-    </row>
-    <row r="103" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="90"/>
-      <c r="B103" s="91" t="s">
+      <c r="C105" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="85" t="s">
+        <v>452</v>
+      </c>
+      <c r="E105" s="85"/>
+    </row>
+    <row r="106" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="96"/>
+      <c r="B106" s="91" t="s">
         <v>382</v>
       </c>
-      <c r="C103" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D103" s="85" t="s">
+      <c r="C106" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D106" s="85" t="s">
+        <v>453</v>
+      </c>
+      <c r="E106" s="85"/>
+    </row>
+    <row r="107" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="96"/>
+      <c r="B107" s="91" t="s">
         <v>383</v>
       </c>
-      <c r="E103" s="85"/>
-    </row>
-    <row r="104" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="90"/>
-      <c r="B104" s="91" t="s">
+      <c r="C107" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D107" s="85" t="s">
         <v>384</v>
       </c>
-      <c r="C104" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D104" s="85" t="s">
-        <v>455</v>
-      </c>
-      <c r="E104" s="85"/>
-    </row>
-    <row r="105" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="90"/>
-      <c r="B105" s="91" t="s">
+      <c r="E107" s="85"/>
+    </row>
+    <row r="108" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="96"/>
+      <c r="B108" s="91" t="s">
         <v>385</v>
       </c>
-      <c r="C105" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D105" s="85" t="s">
-        <v>456</v>
-      </c>
-      <c r="E105" s="85"/>
-    </row>
-    <row r="106" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="90"/>
-      <c r="B106" s="91" t="s">
+      <c r="C108" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D108" s="85" t="s">
         <v>386</v>
       </c>
-      <c r="C106" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D106" s="85" t="s">
-        <v>457</v>
-      </c>
-      <c r="E106" s="85"/>
-    </row>
-    <row r="107" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="90"/>
-      <c r="B107" s="91" t="s">
-        <v>387</v>
-      </c>
-      <c r="C107" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D107" s="85" t="s">
-        <v>388</v>
-      </c>
-      <c r="E107" s="85"/>
-    </row>
-    <row r="108" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="90"/>
-      <c r="B108" s="91" t="s">
-        <v>389</v>
-      </c>
-      <c r="C108" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D108" s="85" t="s">
-        <v>390</v>
-      </c>
       <c r="E108" s="85"/>
     </row>
     <row r="109" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="90"/>
+      <c r="A109" s="96"/>
       <c r="B109" s="91" t="s">
         <v>187</v>
       </c>
@@ -7379,155 +7452,155 @@
         <v>258</v>
       </c>
       <c r="D109" s="85" t="s">
+        <v>387</v>
+      </c>
+      <c r="E109" s="85"/>
+    </row>
+    <row r="110" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="96"/>
+      <c r="B110" s="91" t="s">
+        <v>388</v>
+      </c>
+      <c r="C110" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D110" s="85" t="s">
+        <v>455</v>
+      </c>
+      <c r="E110" s="85"/>
+    </row>
+    <row r="111" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="96"/>
+      <c r="B111" s="91" t="s">
+        <v>372</v>
+      </c>
+      <c r="C111" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D111" s="85" t="s">
+        <v>390</v>
+      </c>
+      <c r="E111" s="85"/>
+    </row>
+    <row r="112" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="96"/>
+      <c r="B112" s="91" t="s">
+        <v>373</v>
+      </c>
+      <c r="C112" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D112" s="85" t="s">
+        <v>469</v>
+      </c>
+      <c r="E112" s="85"/>
+    </row>
+    <row r="113" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="96"/>
+      <c r="B113" s="91" t="s">
         <v>391</v>
       </c>
-      <c r="E109" s="85"/>
-    </row>
-    <row r="110" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="90"/>
-      <c r="B110" s="91" t="s">
+      <c r="C113" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D113" s="85" t="s">
+        <v>471</v>
+      </c>
+      <c r="E113" s="85"/>
+    </row>
+    <row r="114" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="95"/>
+      <c r="B114" s="91" t="s">
         <v>392</v>
       </c>
-      <c r="C110" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D110" s="85" t="s">
-        <v>459</v>
-      </c>
-      <c r="E110" s="85"/>
-    </row>
-    <row r="111" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="90"/>
-      <c r="B111" s="91" t="s">
-        <v>376</v>
-      </c>
-      <c r="C111" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D111" s="85" t="s">
+      <c r="C114" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D114" s="85" t="s">
+        <v>393</v>
+      </c>
+      <c r="E114" s="85"/>
+    </row>
+    <row r="115" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="95"/>
+      <c r="B115" s="91" t="s">
         <v>394</v>
       </c>
-      <c r="E111" s="85"/>
-    </row>
-    <row r="112" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="90"/>
-      <c r="B112" s="91" t="s">
-        <v>377</v>
-      </c>
-      <c r="C112" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D112" s="85" t="s">
-        <v>473</v>
-      </c>
-      <c r="E112" s="85"/>
-    </row>
-    <row r="113" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="90"/>
-      <c r="B113" s="91" t="s">
+      <c r="C115" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D115" s="85" t="s">
         <v>395</v>
       </c>
-      <c r="C113" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D113" s="85" t="s">
-        <v>475</v>
-      </c>
-      <c r="E113" s="85"/>
-    </row>
-    <row r="114" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="90"/>
-      <c r="B114" s="91" t="s">
+      <c r="E115" s="85"/>
+    </row>
+    <row r="116" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="96"/>
+      <c r="B116" s="91" t="s">
         <v>396</v>
       </c>
-      <c r="C114" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D114" s="85" t="s">
+      <c r="C116" s="85" t="s">
+        <v>275</v>
+      </c>
+      <c r="D116" s="85" t="s">
         <v>397</v>
       </c>
-      <c r="E114" s="85"/>
-    </row>
-    <row r="115" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="90"/>
-      <c r="B115" s="91" t="s">
+      <c r="E116" s="85"/>
+    </row>
+    <row r="117" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="98"/>
+      <c r="B117" s="99" t="s">
         <v>398</v>
       </c>
-      <c r="C115" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D115" s="85" t="s">
+      <c r="C117" s="100" t="s">
+        <v>335</v>
+      </c>
+      <c r="D117" s="100" t="s">
         <v>399</v>
       </c>
-      <c r="E115" s="85"/>
-    </row>
-    <row r="116" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="109"/>
-      <c r="B116" s="110" t="s">
+      <c r="E117" s="100"/>
+    </row>
+    <row r="118" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="96"/>
+      <c r="B118" s="91" t="s">
         <v>400</v>
       </c>
-      <c r="C116" s="111" t="s">
-        <v>279</v>
-      </c>
-      <c r="D116" s="111" t="s">
+      <c r="C118" s="85" t="s">
+        <v>275</v>
+      </c>
+      <c r="D118" s="85" t="s">
         <v>401</v>
       </c>
-      <c r="E116" s="111"/>
-    </row>
-    <row r="117" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="90"/>
-      <c r="B117" s="91" t="s">
+      <c r="E118" s="85"/>
+    </row>
+    <row r="119" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="95"/>
+      <c r="B119" s="91" t="s">
         <v>402</v>
       </c>
-      <c r="C117" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D117" s="85" t="s">
+      <c r="C119" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D119" s="85" t="s">
         <v>403</v>
       </c>
-      <c r="E117" s="85"/>
-    </row>
-    <row r="118" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="109"/>
-      <c r="B118" s="110" t="s">
+      <c r="E119" s="85"/>
+    </row>
+    <row r="120" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="95"/>
+      <c r="B120" s="91" t="s">
         <v>404</v>
       </c>
-      <c r="C118" s="111" t="s">
-        <v>279</v>
-      </c>
-      <c r="D118" s="111" t="s">
+      <c r="C120" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D120" s="85" t="s">
         <v>405</v>
       </c>
-      <c r="E118" s="111"/>
-    </row>
-    <row r="119" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="90"/>
-      <c r="B119" s="91" t="s">
-        <v>406</v>
-      </c>
-      <c r="C119" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D119" s="85" t="s">
-        <v>407</v>
-      </c>
-      <c r="E119" s="85"/>
-    </row>
-    <row r="120" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="90"/>
-      <c r="B120" s="91" t="s">
-        <v>408</v>
-      </c>
-      <c r="C120" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D120" s="85" t="s">
-        <v>409</v>
-      </c>
       <c r="E120" s="85"/>
     </row>
     <row r="121" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="90"/>
+      <c r="A121" s="95"/>
       <c r="B121" s="91" t="s">
         <v>188</v>
       </c>
@@ -7535,116 +7608,116 @@
         <v>258</v>
       </c>
       <c r="D121" s="85" t="s">
+        <v>406</v>
+      </c>
+      <c r="E121" s="85"/>
+    </row>
+    <row r="122" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="95"/>
+      <c r="B122" s="91" t="s">
+        <v>407</v>
+      </c>
+      <c r="C122" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D122" s="85" t="s">
+        <v>409</v>
+      </c>
+      <c r="E122" s="85"/>
+    </row>
+    <row r="123" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="95"/>
+      <c r="B123" s="91" t="s">
+        <v>408</v>
+      </c>
+      <c r="C123" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D123" s="85" t="s">
         <v>410</v>
       </c>
-      <c r="E121" s="85"/>
-    </row>
-    <row r="122" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="90"/>
-      <c r="B122" s="91" t="s">
+      <c r="E123" s="85"/>
+    </row>
+    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="96"/>
+      <c r="B124" s="91" t="s">
         <v>411</v>
       </c>
-      <c r="C122" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D122" s="85" t="s">
+      <c r="C124" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D124" s="85" t="s">
+        <v>412</v>
+      </c>
+      <c r="E124" s="85"/>
+    </row>
+    <row r="125" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="96"/>
+      <c r="B125" s="91" t="s">
         <v>413</v>
       </c>
-      <c r="E122" s="85"/>
-    </row>
-    <row r="123" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="90"/>
-      <c r="B123" s="91" t="s">
-        <v>412</v>
-      </c>
-      <c r="C123" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D123" s="85" t="s">
+      <c r="C125" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D125" s="85" t="s">
         <v>414</v>
       </c>
-      <c r="E123" s="85"/>
-    </row>
-    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="90"/>
-      <c r="B124" s="91" t="s">
+      <c r="E125" s="85"/>
+    </row>
+    <row r="126" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="96"/>
+      <c r="B126" s="91" t="s">
         <v>415</v>
       </c>
-      <c r="C124" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D124" s="85" t="s">
+      <c r="C126" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D126" s="85" t="s">
+        <v>459</v>
+      </c>
+      <c r="E126" s="85"/>
+    </row>
+    <row r="127" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="96"/>
+      <c r="B127" s="91" t="s">
         <v>416</v>
       </c>
-      <c r="E124" s="85"/>
-    </row>
-    <row r="125" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="90"/>
-      <c r="B125" s="91" t="s">
+      <c r="C127" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D127" s="85" t="s">
         <v>417</v>
       </c>
-      <c r="C125" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D125" s="85" t="s">
+      <c r="E127" s="85"/>
+    </row>
+    <row r="128" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="96"/>
+      <c r="B128" s="91" t="s">
         <v>418</v>
       </c>
-      <c r="E125" s="85"/>
-    </row>
-    <row r="126" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="90"/>
-      <c r="B126" s="91" t="s">
+      <c r="C128" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D128" s="85" t="s">
         <v>419</v>
       </c>
-      <c r="C126" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D126" s="85" t="s">
-        <v>463</v>
-      </c>
-      <c r="E126" s="85"/>
-    </row>
-    <row r="127" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="90"/>
-      <c r="B127" s="91" t="s">
+      <c r="E128" s="85"/>
+    </row>
+    <row r="129" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="96"/>
+      <c r="B129" s="91" t="s">
         <v>420</v>
       </c>
-      <c r="C127" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D127" s="85" t="s">
+      <c r="C129" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D129" s="85" t="s">
         <v>421</v>
       </c>
-      <c r="E127" s="85"/>
-    </row>
-    <row r="128" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="90"/>
-      <c r="B128" s="91" t="s">
-        <v>422</v>
-      </c>
-      <c r="C128" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D128" s="85" t="s">
-        <v>423</v>
-      </c>
-      <c r="E128" s="85"/>
-    </row>
-    <row r="129" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="90"/>
-      <c r="B129" s="91" t="s">
-        <v>424</v>
-      </c>
-      <c r="C129" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D129" s="85" t="s">
-        <v>425</v>
-      </c>
       <c r="E129" s="85"/>
     </row>
     <row r="130" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="90"/>
+      <c r="A130" s="96"/>
       <c r="B130" s="91" t="s">
         <v>189</v>
       </c>
@@ -7652,12 +7725,12 @@
         <v>258</v>
       </c>
       <c r="D130" s="85" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E130" s="85"/>
     </row>
     <row r="131" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="90"/>
+      <c r="A131" s="96"/>
       <c r="B131" s="91" t="s">
         <v>190</v>
       </c>
@@ -7665,470 +7738,586 @@
         <v>258</v>
       </c>
       <c r="D131" s="85" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E131" s="85"/>
     </row>
     <row r="132" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="90"/>
+      <c r="A132" s="96"/>
       <c r="B132" s="91" t="s">
+        <v>423</v>
+      </c>
+      <c r="C132" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D132" s="85" t="s">
+        <v>424</v>
+      </c>
+      <c r="E132" s="85"/>
+    </row>
+    <row r="133" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="96"/>
+      <c r="B133" s="91" t="s">
+        <v>425</v>
+      </c>
+      <c r="C133" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D133" s="85" t="s">
+        <v>426</v>
+      </c>
+      <c r="E133" s="85"/>
+    </row>
+    <row r="134" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="96"/>
+      <c r="B134" s="91" t="s">
         <v>427</v>
       </c>
-      <c r="C132" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D132" s="85" t="s">
+      <c r="C134" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D134" s="85" t="s">
+        <v>461</v>
+      </c>
+      <c r="E134" s="85"/>
+    </row>
+    <row r="135" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="96"/>
+      <c r="B135" s="91" t="s">
         <v>428</v>
       </c>
-      <c r="E132" s="85"/>
-    </row>
-    <row r="133" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="90"/>
-      <c r="B133" s="91" t="s">
+      <c r="C135" s="85" t="s">
+        <v>269</v>
+      </c>
+      <c r="D135" s="85" t="s">
         <v>429</v>
       </c>
-      <c r="C133" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D133" s="85" t="s">
+      <c r="E135" s="85"/>
+    </row>
+    <row r="136" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="96"/>
+      <c r="B136" s="91" t="s">
         <v>430</v>
       </c>
-      <c r="E133" s="85"/>
-    </row>
-    <row r="134" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="90"/>
-      <c r="B134" s="91" t="s">
+      <c r="C136" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D136" s="85" t="s">
         <v>431</v>
       </c>
-      <c r="C134" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D134" s="85" t="s">
-        <v>465</v>
-      </c>
-      <c r="E134" s="85"/>
-    </row>
-    <row r="135" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="90"/>
-      <c r="B135" s="91" t="s">
+      <c r="E136" s="85"/>
+    </row>
+    <row r="137" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="96"/>
+      <c r="B137" s="91" t="s">
         <v>432</v>
       </c>
-      <c r="C135" s="85" t="s">
-        <v>272</v>
-      </c>
-      <c r="D135" s="85" t="s">
+      <c r="C137" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D137" s="85" t="s">
+        <v>520</v>
+      </c>
+      <c r="E137" s="85"/>
+    </row>
+    <row r="138" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="96"/>
+      <c r="B138" s="91" t="s">
         <v>433</v>
       </c>
-      <c r="E135" s="85"/>
-    </row>
-    <row r="136" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="90"/>
-      <c r="B136" s="91" t="s">
+      <c r="C138" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D138" s="85" t="s">
+        <v>463</v>
+      </c>
+      <c r="E138" s="85"/>
+    </row>
+    <row r="139" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="96"/>
+      <c r="B139" s="91" t="s">
         <v>434</v>
       </c>
-      <c r="C136" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D136" s="85" t="s">
+      <c r="C139" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D139" s="85" t="s">
         <v>435</v>
       </c>
-      <c r="E136" s="85"/>
-    </row>
-    <row r="137" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="90"/>
-      <c r="B137" s="91" t="s">
+      <c r="E139" s="85"/>
+    </row>
+    <row r="140" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="96"/>
+      <c r="B140" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="C137" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D137" s="85" t="s">
+      <c r="C140" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D140" s="85" t="s">
+        <v>464</v>
+      </c>
+      <c r="E140" s="85"/>
+    </row>
+    <row r="141" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="96"/>
+      <c r="B141" s="91" t="s">
+        <v>437</v>
+      </c>
+      <c r="C141" s="85" t="s">
+        <v>275</v>
+      </c>
+      <c r="D141" s="85" t="s">
+        <v>438</v>
+      </c>
+      <c r="E141" s="85"/>
+    </row>
+    <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="95"/>
+      <c r="B142" s="91" t="s">
+        <v>456</v>
+      </c>
+      <c r="C142" s="85" t="s">
+        <v>269</v>
+      </c>
+      <c r="D142" s="85" t="s">
+        <v>457</v>
+      </c>
+      <c r="E142" s="85"/>
+    </row>
+    <row r="143" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="98"/>
+      <c r="B143" s="99" t="s">
+        <v>466</v>
+      </c>
+      <c r="C143" s="100" t="s">
+        <v>301</v>
+      </c>
+      <c r="D143" s="100" t="s">
+        <v>467</v>
+      </c>
+      <c r="E143" s="100"/>
+    </row>
+    <row r="144" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="96"/>
+      <c r="B144" s="91" t="s">
+        <v>473</v>
+      </c>
+      <c r="C144" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D144" s="85" t="s">
+        <v>474</v>
+      </c>
+      <c r="E144" s="85"/>
+    </row>
+    <row r="145" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="96"/>
+      <c r="B145" s="91" t="s">
+        <v>476</v>
+      </c>
+      <c r="C145" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D145" s="85" t="s">
+        <v>477</v>
+      </c>
+      <c r="E145" s="85"/>
+    </row>
+    <row r="146" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="96"/>
+      <c r="B146" s="91" t="s">
+        <v>478</v>
+      </c>
+      <c r="C146" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D146" s="85" t="s">
+        <v>479</v>
+      </c>
+      <c r="E146" s="85"/>
+    </row>
+    <row r="147" spans="1:5" s="94" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="103"/>
+      <c r="B147" s="92" t="s">
+        <v>480</v>
+      </c>
+      <c r="C147" s="93" t="s">
+        <v>335</v>
+      </c>
+      <c r="D147" s="93" t="s">
+        <v>481</v>
+      </c>
+      <c r="E147" s="93"/>
+    </row>
+    <row r="148" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="96"/>
+      <c r="B148" s="91" t="s">
+        <v>482</v>
+      </c>
+      <c r="C148" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D148" s="85" t="s">
+        <v>483</v>
+      </c>
+      <c r="E148" s="85"/>
+    </row>
+    <row r="149" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="96"/>
+      <c r="B149" s="91" t="s">
+        <v>485</v>
+      </c>
+      <c r="C149" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D149" s="85" t="s">
+        <v>486</v>
+      </c>
+      <c r="E149" s="85"/>
+    </row>
+    <row r="150" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="96"/>
+      <c r="B150" s="91" t="s">
+        <v>487</v>
+      </c>
+      <c r="C150" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D150" s="85" t="s">
+        <v>488</v>
+      </c>
+      <c r="E150" s="85"/>
+    </row>
+    <row r="151" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="96"/>
+      <c r="B151" s="91" t="s">
+        <v>490</v>
+      </c>
+      <c r="C151" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D151" s="85" t="s">
+        <v>489</v>
+      </c>
+      <c r="E151" s="85"/>
+    </row>
+    <row r="152" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="96"/>
+      <c r="B152" s="91" t="s">
+        <v>491</v>
+      </c>
+      <c r="C152" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D152" s="85" t="s">
+        <v>492</v>
+      </c>
+      <c r="E152" s="85"/>
+    </row>
+    <row r="153" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="96"/>
+      <c r="B153" s="91" t="s">
+        <v>493</v>
+      </c>
+      <c r="C153" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D153" s="85" t="s">
+        <v>501</v>
+      </c>
+      <c r="E153" s="85"/>
+    </row>
+    <row r="154" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="95"/>
+      <c r="B154" s="91" t="s">
+        <v>494</v>
+      </c>
+      <c r="C154" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D154" s="85" t="s">
+        <v>502</v>
+      </c>
+      <c r="E154" s="85"/>
+    </row>
+    <row r="155" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="95"/>
+      <c r="B155" s="91" t="s">
+        <v>495</v>
+      </c>
+      <c r="C155" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D155" s="85" t="s">
+        <v>503</v>
+      </c>
+      <c r="E155" s="85"/>
+    </row>
+    <row r="156" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="95"/>
+      <c r="B156" s="91" t="s">
+        <v>496</v>
+      </c>
+      <c r="C156" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D156" s="85" t="s">
+        <v>504</v>
+      </c>
+      <c r="E156" s="85"/>
+    </row>
+    <row r="157" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="95"/>
+      <c r="B157" s="91" t="s">
+        <v>497</v>
+      </c>
+      <c r="C157" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D157" s="85" t="s">
+        <v>505</v>
+      </c>
+      <c r="E157" s="85"/>
+    </row>
+    <row r="158" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="95"/>
+      <c r="B158" s="91" t="s">
+        <v>498</v>
+      </c>
+      <c r="C158" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D158" s="85" t="s">
+        <v>506</v>
+      </c>
+      <c r="E158" s="85"/>
+    </row>
+    <row r="159" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="95"/>
+      <c r="B159" s="91" t="s">
+        <v>499</v>
+      </c>
+      <c r="C159" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D159" s="85" t="s">
+        <v>507</v>
+      </c>
+      <c r="E159" s="85"/>
+    </row>
+    <row r="160" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="95"/>
+      <c r="B160" s="91" t="s">
+        <v>500</v>
+      </c>
+      <c r="C160" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D160" s="85" t="s">
+        <v>508</v>
+      </c>
+      <c r="E160" s="85"/>
+    </row>
+    <row r="161" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="95"/>
+      <c r="B161" s="91" t="s">
+        <v>509</v>
+      </c>
+      <c r="C161" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D161" s="85" t="s">
+        <v>510</v>
+      </c>
+      <c r="E161" s="85"/>
+    </row>
+    <row r="162" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="96"/>
+      <c r="B162" s="91" t="s">
+        <v>511</v>
+      </c>
+      <c r="C162" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D162" s="85" t="s">
+        <v>514</v>
+      </c>
+      <c r="E162" s="85"/>
+    </row>
+    <row r="163" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="96"/>
+      <c r="B163" s="91" t="s">
+        <v>512</v>
+      </c>
+      <c r="C163" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D163" s="85" t="s">
+        <v>515</v>
+      </c>
+      <c r="E163" s="85"/>
+    </row>
+    <row r="164" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="96"/>
+      <c r="B164" s="91" t="s">
+        <v>513</v>
+      </c>
+      <c r="C164" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D164" s="85" t="s">
+        <v>516</v>
+      </c>
+      <c r="E164" s="85"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="96"/>
+      <c r="B165" s="83" t="s">
+        <v>521</v>
+      </c>
+      <c r="C165" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D165" s="84" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="96"/>
+      <c r="B166" s="91" t="s">
+        <v>522</v>
+      </c>
+      <c r="C166" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D166" s="85" t="s">
+        <v>523</v>
+      </c>
+      <c r="E166" s="85"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="96"/>
+      <c r="B167" s="83" t="s">
         <v>524</v>
       </c>
-      <c r="E137" s="85"/>
-    </row>
-    <row r="138" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="90"/>
-      <c r="B138" s="91" t="s">
-        <v>437</v>
-      </c>
-      <c r="C138" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D138" s="85" t="s">
-        <v>467</v>
-      </c>
-      <c r="E138" s="85"/>
-    </row>
-    <row r="139" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="90"/>
-      <c r="B139" s="91" t="s">
-        <v>438</v>
-      </c>
-      <c r="C139" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D139" s="85" t="s">
-        <v>439</v>
-      </c>
-      <c r="E139" s="85"/>
-    </row>
-    <row r="140" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="90"/>
-      <c r="B140" s="91" t="s">
-        <v>440</v>
-      </c>
-      <c r="C140" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D140" s="85" t="s">
-        <v>468</v>
-      </c>
-      <c r="E140" s="85"/>
-    </row>
-    <row r="141" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="90"/>
-      <c r="B141" s="91" t="s">
-        <v>441</v>
-      </c>
-      <c r="C141" s="85" t="s">
-        <v>279</v>
-      </c>
-      <c r="D141" s="85" t="s">
-        <v>442</v>
-      </c>
-      <c r="E141" s="85"/>
-    </row>
-    <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="90"/>
-      <c r="B142" s="91" t="s">
-        <v>460</v>
-      </c>
-      <c r="C142" s="85" t="s">
-        <v>272</v>
-      </c>
-      <c r="D142" s="85" t="s">
-        <v>461</v>
-      </c>
-      <c r="E142" s="85"/>
-    </row>
-    <row r="143" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="90"/>
-      <c r="B143" s="91" t="s">
-        <v>470</v>
-      </c>
-      <c r="C143" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D143" s="85" t="s">
-        <v>471</v>
-      </c>
-      <c r="E143" s="85"/>
-    </row>
-    <row r="144" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="90"/>
-      <c r="B144" s="91" t="s">
-        <v>477</v>
-      </c>
-      <c r="C144" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D144" s="85" t="s">
-        <v>478</v>
-      </c>
-      <c r="E144" s="85"/>
-    </row>
-    <row r="145" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="90"/>
-      <c r="B145" s="91" t="s">
-        <v>480</v>
-      </c>
-      <c r="C145" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D145" s="85" t="s">
-        <v>481</v>
-      </c>
-      <c r="E145" s="85"/>
-    </row>
-    <row r="146" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="90"/>
-      <c r="B146" s="91" t="s">
-        <v>482</v>
-      </c>
-      <c r="C146" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D146" s="85" t="s">
-        <v>483</v>
-      </c>
-      <c r="E146" s="85"/>
-    </row>
-    <row r="147" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="103"/>
-      <c r="B147" s="104" t="s">
-        <v>484</v>
-      </c>
-      <c r="C147" s="105" t="s">
-        <v>339</v>
-      </c>
-      <c r="D147" s="105" t="s">
-        <v>485</v>
-      </c>
-      <c r="E147" s="105"/>
-    </row>
-    <row r="148" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="90"/>
-      <c r="B148" s="91" t="s">
-        <v>486</v>
-      </c>
-      <c r="C148" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D148" s="85" t="s">
-        <v>487</v>
-      </c>
-      <c r="E148" s="85"/>
-    </row>
-    <row r="149" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="90"/>
-      <c r="B149" s="91" t="s">
-        <v>489</v>
-      </c>
-      <c r="C149" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D149" s="85" t="s">
-        <v>490</v>
-      </c>
-      <c r="E149" s="85"/>
-    </row>
-    <row r="150" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="90"/>
-      <c r="B150" s="91" t="s">
-        <v>491</v>
-      </c>
-      <c r="C150" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D150" s="85" t="s">
-        <v>492</v>
-      </c>
-      <c r="E150" s="85"/>
-    </row>
-    <row r="151" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="90"/>
-      <c r="B151" s="91" t="s">
-        <v>494</v>
-      </c>
-      <c r="C151" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D151" s="85" t="s">
-        <v>493</v>
-      </c>
-      <c r="E151" s="85"/>
-    </row>
-    <row r="152" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="90"/>
-      <c r="B152" s="91" t="s">
-        <v>495</v>
-      </c>
-      <c r="C152" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D152" s="85" t="s">
-        <v>496</v>
-      </c>
-      <c r="E152" s="85"/>
-    </row>
-    <row r="153" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="90"/>
-      <c r="B153" s="91" t="s">
-        <v>497</v>
-      </c>
-      <c r="C153" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D153" s="85" t="s">
-        <v>505</v>
-      </c>
-      <c r="E153" s="85"/>
-    </row>
-    <row r="154" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="90"/>
-      <c r="B154" s="91" t="s">
-        <v>498</v>
-      </c>
-      <c r="C154" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D154" s="85" t="s">
-        <v>506</v>
-      </c>
-      <c r="E154" s="85"/>
-    </row>
-    <row r="155" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="90"/>
-      <c r="B155" s="91" t="s">
-        <v>499</v>
-      </c>
-      <c r="C155" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D155" s="85" t="s">
-        <v>507</v>
-      </c>
-      <c r="E155" s="85"/>
-    </row>
-    <row r="156" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="90"/>
-      <c r="B156" s="91" t="s">
-        <v>500</v>
-      </c>
-      <c r="C156" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D156" s="85" t="s">
-        <v>508</v>
-      </c>
-      <c r="E156" s="85"/>
-    </row>
-    <row r="157" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="90"/>
-      <c r="B157" s="91" t="s">
-        <v>501</v>
-      </c>
-      <c r="C157" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D157" s="85" t="s">
-        <v>509</v>
-      </c>
-      <c r="E157" s="85"/>
-    </row>
-    <row r="158" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="90"/>
-      <c r="B158" s="91" t="s">
-        <v>502</v>
-      </c>
-      <c r="C158" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D158" s="85" t="s">
-        <v>510</v>
-      </c>
-      <c r="E158" s="85"/>
-    </row>
-    <row r="159" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="90"/>
-      <c r="B159" s="91" t="s">
-        <v>503</v>
-      </c>
-      <c r="C159" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D159" s="85" t="s">
-        <v>511</v>
-      </c>
-      <c r="E159" s="85"/>
-    </row>
-    <row r="160" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="90"/>
-      <c r="B160" s="91" t="s">
-        <v>504</v>
-      </c>
-      <c r="C160" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D160" s="85" t="s">
-        <v>512</v>
-      </c>
-      <c r="E160" s="85"/>
-    </row>
-    <row r="161" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="90"/>
-      <c r="B161" s="91" t="s">
-        <v>513</v>
-      </c>
-      <c r="C161" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D161" s="85" t="s">
-        <v>514</v>
-      </c>
-      <c r="E161" s="85"/>
-    </row>
-    <row r="162" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="90"/>
-      <c r="B162" s="91" t="s">
-        <v>515</v>
-      </c>
-      <c r="C162" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D162" s="85" t="s">
-        <v>518</v>
-      </c>
-      <c r="E162" s="85"/>
-    </row>
-    <row r="163" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="90"/>
-      <c r="B163" s="91" t="s">
-        <v>516</v>
-      </c>
-      <c r="C163" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D163" s="85" t="s">
-        <v>519</v>
-      </c>
-      <c r="E163" s="85"/>
-    </row>
-    <row r="164" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="90"/>
-      <c r="B164" s="91" t="s">
-        <v>517</v>
-      </c>
-      <c r="C164" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D164" s="85" t="s">
-        <v>520</v>
-      </c>
-      <c r="E164" s="85"/>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B165" s="83" t="s">
+      <c r="C167" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D167" s="84" t="s">
         <v>525</v>
       </c>
-      <c r="C165" s="84" t="s">
-        <v>339</v>
-      </c>
-      <c r="D165" s="84" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B166" s="83" t="s">
+    </row>
+    <row r="168" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="96"/>
+      <c r="B168" s="91" t="s">
         <v>526</v>
       </c>
-      <c r="C166" s="84" t="s">
-        <v>339</v>
-      </c>
-      <c r="D166" s="84" t="s">
+      <c r="C168" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D168" s="85" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B167" s="83" t="s">
+      <c r="E168" s="85"/>
+    </row>
+    <row r="169" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="96"/>
+      <c r="B169" s="91" t="s">
         <v>528</v>
       </c>
-      <c r="C167" s="84" t="s">
-        <v>339</v>
-      </c>
-      <c r="D167" s="84" t="s">
+      <c r="C169" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D169" s="85" t="s">
         <v>529</v>
+      </c>
+      <c r="E169" s="85"/>
+    </row>
+    <row r="170" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="96"/>
+      <c r="B170" s="91" t="s">
+        <v>530</v>
+      </c>
+      <c r="C170" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D170" s="85" t="s">
+        <v>531</v>
+      </c>
+      <c r="E170" s="85"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="95"/>
+      <c r="B171" s="83" t="s">
+        <v>532</v>
+      </c>
+      <c r="C171" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D171" s="84" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="96"/>
+      <c r="B172" s="91" t="s">
+        <v>534</v>
+      </c>
+      <c r="C172" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D172" s="85" t="s">
+        <v>535</v>
+      </c>
+      <c r="E172" s="85"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="96"/>
+      <c r="B173" s="83" t="s">
+        <v>542</v>
+      </c>
+      <c r="C173" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D173" s="84" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="96"/>
+      <c r="B174" s="83" t="s">
+        <v>544</v>
+      </c>
+      <c r="C174" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D174" s="84" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="96"/>
+      <c r="B175" s="83" t="s">
+        <v>545</v>
+      </c>
+      <c r="C175" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D175" s="84" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="96"/>
+      <c r="B176" s="83" t="s">
+        <v>547</v>
+      </c>
+      <c r="C176" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D176" s="84" t="s">
+        <v>548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>